<commit_message>
fixed formatting of column "ready" removed wrong file climate_indices_CV22.csv
</commit_message>
<xml_diff>
--- a/climate_indices_CV22.xlsx
+++ b/climate_indices_CV22.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7794" uniqueCount="1128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7708" uniqueCount="1128">
   <si>
     <t xml:space="preserve">VarName</t>
   </si>
@@ -3841,7 +3841,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="94">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4126,15 +4126,31 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4297,7 +4313,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
-      <selection pane="bottomRight" activeCell="A27" activeCellId="0" sqref="15:36"/>
+      <selection pane="bottomRight" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18054,7 +18070,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="15:36"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18326,7 +18342,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="15:36 B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18720,7 +18736,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AS126"/>
@@ -18730,20 +18746,20 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B36" activeCellId="0" sqref="15:36"/>
+      <selection pane="bottomRight" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="70" width="13.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="70" width="7.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="71" width="7.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="70" width="11.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="70" width="7.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="70" width="9.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="70" width="24.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="71" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="72" width="23.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="72" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="72" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="71" width="23.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="71" width="12.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="70" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="70" width="9.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="70" width="52.14"/>
@@ -18782,7 +18798,7 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -18896,8 +18912,8 @@
       <c r="A2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>34</v>
+      <c r="B2" s="10" t="n">
+        <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>35</v>
@@ -19000,8 +19016,8 @@
       <c r="A3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>34</v>
+      <c r="B3" s="14" t="n">
+        <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>35</v>
@@ -19104,8 +19120,8 @@
       <c r="A4" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>34</v>
+      <c r="B4" s="14" t="n">
+        <v>1</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>35</v>
@@ -19206,8 +19222,8 @@
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>34</v>
+      <c r="B5" s="14" t="n">
+        <v>1</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>35</v>
@@ -19308,8 +19324,8 @@
       <c r="A6" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>34</v>
+      <c r="B6" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>35</v>
@@ -19410,8 +19426,8 @@
       <c r="A7" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>34</v>
+      <c r="B7" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>35</v>
@@ -19512,8 +19528,8 @@
       <c r="A8" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>34</v>
+      <c r="B8" s="14" t="n">
+        <v>1</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>35</v>
@@ -19614,8 +19630,8 @@
       <c r="A9" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>34</v>
+      <c r="B9" s="14" t="n">
+        <v>1</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>35</v>
@@ -19718,8 +19734,8 @@
       <c r="A10" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>34</v>
+      <c r="B10" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>35</v>
@@ -19822,8 +19838,8 @@
       <c r="A11" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>34</v>
+      <c r="B11" s="14" t="n">
+        <v>1</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>35</v>
@@ -19926,8 +19942,8 @@
       <c r="A12" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>34</v>
+      <c r="B12" s="14" t="n">
+        <v>1</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>35</v>
@@ -20030,8 +20046,8 @@
       <c r="A13" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>34</v>
+      <c r="B13" s="14" t="n">
+        <v>1</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>35</v>
@@ -20134,8 +20150,8 @@
       <c r="A14" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>34</v>
+      <c r="B14" s="14" t="n">
+        <v>1</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>35</v>
@@ -20238,7 +20254,7 @@
       <c r="A15" s="19" t="s">
         <v>684</v>
       </c>
-      <c r="B15" s="19" t="n">
+      <c r="B15" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C15" s="19" t="s">
@@ -20342,7 +20358,7 @@
       <c r="A16" s="19" t="s">
         <v>685</v>
       </c>
-      <c r="B16" s="19" t="n">
+      <c r="B16" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C16" s="19" t="s">
@@ -20442,11 +20458,11 @@
       <c r="AQ16" s="20"/>
       <c r="AR16" s="20"/>
     </row>
-    <row r="17" s="73" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="73" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="s">
         <v>686</v>
       </c>
-      <c r="B17" s="23" t="n">
+      <c r="B17" s="26" t="n">
         <v>0</v>
       </c>
       <c r="C17" s="24" t="s">
@@ -20546,11 +20562,11 @@
       <c r="AQ17" s="24"/>
       <c r="AR17" s="24"/>
     </row>
-    <row r="18" s="73" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="73" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
         <v>687</v>
       </c>
-      <c r="B18" s="23" t="n">
+      <c r="B18" s="26" t="n">
         <v>0</v>
       </c>
       <c r="C18" s="24" t="s">
@@ -20654,7 +20670,7 @@
       <c r="A19" s="19" t="s">
         <v>688</v>
       </c>
-      <c r="B19" s="19" t="n">
+      <c r="B19" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C19" s="19" t="s">
@@ -20758,7 +20774,7 @@
       <c r="A20" s="19" t="s">
         <v>689</v>
       </c>
-      <c r="B20" s="19" t="n">
+      <c r="B20" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C20" s="19" t="s">
@@ -20858,11 +20874,11 @@
       <c r="AQ20" s="20"/>
       <c r="AR20" s="20"/>
     </row>
-    <row r="21" s="73" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="73" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="19" t="s">
         <v>690</v>
       </c>
-      <c r="B21" s="19" t="n">
+      <c r="B21" s="22" t="n">
         <v>0</v>
       </c>
       <c r="C21" s="19" t="s">
@@ -20962,11 +20978,11 @@
       <c r="AQ21" s="19"/>
       <c r="AR21" s="19"/>
     </row>
-    <row r="22" s="73" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" s="73" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="23" t="s">
         <v>691</v>
       </c>
-      <c r="B22" s="23" t="n">
+      <c r="B22" s="26" t="n">
         <v>0</v>
       </c>
       <c r="C22" s="24" t="s">
@@ -21070,7 +21086,7 @@
       <c r="A23" s="19" t="s">
         <v>692</v>
       </c>
-      <c r="B23" s="19" t="n">
+      <c r="B23" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="19" t="s">
@@ -21174,7 +21190,7 @@
       <c r="A24" s="19" t="s">
         <v>693</v>
       </c>
-      <c r="B24" s="19" t="n">
+      <c r="B24" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C24" s="19" t="s">
@@ -21274,11 +21290,11 @@
       <c r="AQ24" s="20"/>
       <c r="AR24" s="20"/>
     </row>
-    <row r="25" s="73" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" s="73" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="19" t="s">
         <v>694</v>
       </c>
-      <c r="B25" s="19" t="n">
+      <c r="B25" s="22" t="n">
         <v>0</v>
       </c>
       <c r="C25" s="19" t="s">
@@ -21378,11 +21394,11 @@
       <c r="AQ25" s="19"/>
       <c r="AR25" s="19"/>
     </row>
-    <row r="26" s="73" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" s="73" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
         <v>695</v>
       </c>
-      <c r="B26" s="23" t="n">
+      <c r="B26" s="26" t="n">
         <v>0</v>
       </c>
       <c r="C26" s="24" t="s">
@@ -21486,7 +21502,7 @@
       <c r="A27" s="19" t="s">
         <v>696</v>
       </c>
-      <c r="B27" s="19" t="n">
+      <c r="B27" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -21590,7 +21606,7 @@
       <c r="A28" s="19" t="s">
         <v>697</v>
       </c>
-      <c r="B28" s="19" t="n">
+      <c r="B28" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C28" s="19" t="s">
@@ -21690,11 +21706,11 @@
       <c r="AQ28" s="20"/>
       <c r="AR28" s="20"/>
     </row>
-    <row r="29" s="73" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" s="73" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="23" t="s">
         <v>698</v>
       </c>
-      <c r="B29" s="23" t="n">
+      <c r="B29" s="26" t="n">
         <v>0</v>
       </c>
       <c r="C29" s="24" t="s">
@@ -21794,11 +21810,11 @@
       <c r="AQ29" s="24"/>
       <c r="AR29" s="24"/>
     </row>
-    <row r="30" s="73" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="73" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="23" t="s">
         <v>699</v>
       </c>
-      <c r="B30" s="23" t="n">
+      <c r="B30" s="26" t="n">
         <v>0</v>
       </c>
       <c r="C30" s="24" t="s">
@@ -21902,7 +21918,7 @@
       <c r="A31" s="19" t="s">
         <v>700</v>
       </c>
-      <c r="B31" s="19" t="n">
+      <c r="B31" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C31" s="19" t="s">
@@ -22006,7 +22022,7 @@
       <c r="A32" s="19" t="s">
         <v>702</v>
       </c>
-      <c r="B32" s="19" t="n">
+      <c r="B32" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C32" s="19" t="s">
@@ -22106,11 +22122,11 @@
       <c r="AQ32" s="20"/>
       <c r="AR32" s="20"/>
     </row>
-    <row r="33" s="73" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" s="73" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="23" t="s">
         <v>703</v>
       </c>
-      <c r="B33" s="23" t="n">
+      <c r="B33" s="26" t="n">
         <v>0</v>
       </c>
       <c r="C33" s="23" t="s">
@@ -22210,11 +22226,11 @@
       <c r="AQ33" s="24"/>
       <c r="AR33" s="24"/>
     </row>
-    <row r="34" s="73" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" s="73" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="23" t="s">
         <v>704</v>
       </c>
-      <c r="B34" s="23" t="n">
+      <c r="B34" s="26" t="n">
         <v>0</v>
       </c>
       <c r="C34" s="23" t="s">
@@ -22318,7 +22334,7 @@
       <c r="A35" s="19" t="s">
         <v>705</v>
       </c>
-      <c r="B35" s="19" t="n">
+      <c r="B35" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -22422,7 +22438,7 @@
       <c r="A36" s="19" t="s">
         <v>706</v>
       </c>
-      <c r="B36" s="19" t="n">
+      <c r="B36" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C36" s="19" t="s">
@@ -22522,11 +22538,11 @@
       <c r="AQ36" s="20"/>
       <c r="AR36" s="20"/>
     </row>
-    <row r="37" s="73" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" s="73" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="23" t="s">
         <v>707</v>
       </c>
-      <c r="B37" s="23" t="n">
+      <c r="B37" s="26" t="n">
         <v>0</v>
       </c>
       <c r="C37" s="23" t="s">
@@ -22626,11 +22642,11 @@
       <c r="AQ37" s="24"/>
       <c r="AR37" s="24"/>
     </row>
-    <row r="38" s="73" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" s="73" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="23" t="s">
         <v>708</v>
       </c>
-      <c r="B38" s="23" t="n">
+      <c r="B38" s="26" t="n">
         <v>0</v>
       </c>
       <c r="C38" s="23" t="s">
@@ -22730,12 +22746,12 @@
       <c r="AQ38" s="24"/>
       <c r="AR38" s="24"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="B39" s="15" t="s">
-        <v>246</v>
+      <c r="B39" s="17" t="n">
+        <v>0</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>247</v>
@@ -22842,12 +22858,12 @@
       <c r="AQ39" s="15"/>
       <c r="AR39" s="15"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="B40" s="33" t="s">
-        <v>246</v>
+      <c r="B40" s="74" t="n">
+        <v>0</v>
       </c>
       <c r="C40" s="33" t="s">
         <v>247</v>
@@ -22954,12 +22970,12 @@
       <c r="AQ40" s="20"/>
       <c r="AR40" s="20"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="33" t="s">
         <v>269</v>
       </c>
-      <c r="B41" s="33" t="s">
-        <v>246</v>
+      <c r="B41" s="74" t="n">
+        <v>0</v>
       </c>
       <c r="C41" s="33" t="s">
         <v>247</v>
@@ -23066,12 +23082,12 @@
       <c r="AQ41" s="20"/>
       <c r="AR41" s="20"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="33" t="s">
         <v>274</v>
       </c>
-      <c r="B42" s="33" t="s">
-        <v>246</v>
+      <c r="B42" s="74" t="n">
+        <v>0</v>
       </c>
       <c r="C42" s="33" t="s">
         <v>247</v>
@@ -23182,8 +23198,8 @@
       <c r="A43" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="B43" s="15" t="s">
-        <v>34</v>
+      <c r="B43" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>35</v>
@@ -23287,8 +23303,8 @@
       <c r="A44" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="B44" s="15" t="s">
-        <v>34</v>
+      <c r="B44" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>35</v>
@@ -23392,8 +23408,8 @@
       <c r="A45" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="B45" s="15" t="s">
-        <v>34</v>
+      <c r="B45" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>35</v>
@@ -23497,8 +23513,8 @@
       <c r="A46" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="B46" s="15" t="s">
-        <v>34</v>
+      <c r="B46" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>35</v>
@@ -23602,7 +23618,7 @@
       <c r="A47" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="B47" s="19" t="n">
+      <c r="B47" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C47" s="19" t="s">
@@ -23707,7 +23723,7 @@
       <c r="A48" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="B48" s="19" t="n">
+      <c r="B48" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C48" s="19" t="s">
@@ -23812,7 +23828,7 @@
       <c r="A49" s="19" t="s">
         <v>311</v>
       </c>
-      <c r="B49" s="19" t="n">
+      <c r="B49" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C49" s="19" t="s">
@@ -23917,7 +23933,7 @@
       <c r="A50" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="B50" s="19" t="n">
+      <c r="B50" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C50" s="19" t="s">
@@ -24022,7 +24038,7 @@
       <c r="A51" s="19" t="s">
         <v>317</v>
       </c>
-      <c r="B51" s="19" t="n">
+      <c r="B51" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C51" s="19" t="s">
@@ -24127,7 +24143,7 @@
       <c r="A52" s="19" t="s">
         <v>322</v>
       </c>
-      <c r="B52" s="19" t="n">
+      <c r="B52" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C52" s="19" t="s">
@@ -24232,7 +24248,7 @@
       <c r="A53" s="19" t="s">
         <v>326</v>
       </c>
-      <c r="B53" s="19" t="n">
+      <c r="B53" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C53" s="19" t="s">
@@ -24337,8 +24353,8 @@
       <c r="A54" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="B54" s="20" t="s">
-        <v>34</v>
+      <c r="B54" s="22" t="n">
+        <v>1</v>
       </c>
       <c r="C54" s="19" t="s">
         <v>35</v>
@@ -24442,7 +24458,7 @@
       <c r="A55" s="19" t="s">
         <v>332</v>
       </c>
-      <c r="B55" s="19" t="n">
+      <c r="B55" s="22" t="n">
         <v>1</v>
       </c>
       <c r="C55" s="19" t="s">
@@ -24543,12 +24559,12 @@
         <v>319</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="15" t="s">
         <v>337</v>
       </c>
-      <c r="B56" s="39" t="s">
-        <v>246</v>
+      <c r="B56" s="75" t="n">
+        <v>0</v>
       </c>
       <c r="C56" s="15" t="s">
         <v>247</v>
@@ -24651,12 +24667,12 @@
       <c r="AQ56" s="15"/>
       <c r="AR56" s="15"/>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11" t="s">
         <v>834</v>
       </c>
-      <c r="B57" s="40" t="s">
-        <v>246</v>
+      <c r="B57" s="76" t="n">
+        <v>0</v>
       </c>
       <c r="C57" s="11" t="s">
         <v>247</v>
@@ -24759,12 +24775,12 @@
       <c r="AQ57" s="11"/>
       <c r="AR57" s="11"/>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="15" t="s">
         <v>355</v>
       </c>
-      <c r="B58" s="39" t="s">
-        <v>246</v>
+      <c r="B58" s="75" t="n">
+        <v>0</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>247</v>
@@ -24867,12 +24883,12 @@
       <c r="AQ58" s="15"/>
       <c r="AR58" s="15"/>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="11" t="s">
         <v>837</v>
       </c>
-      <c r="B59" s="40" t="s">
-        <v>246</v>
+      <c r="B59" s="76" t="n">
+        <v>0</v>
       </c>
       <c r="C59" s="11" t="s">
         <v>247</v>
@@ -24975,12 +24991,12 @@
       <c r="AQ59" s="11"/>
       <c r="AR59" s="11"/>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="B60" s="40" t="s">
-        <v>246</v>
+      <c r="B60" s="76" t="n">
+        <v>0</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>247</v>
@@ -25083,12 +25099,12 @@
       <c r="AQ60" s="11"/>
       <c r="AR60" s="11"/>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="B61" s="39" t="s">
-        <v>246</v>
+      <c r="B61" s="75" t="n">
+        <v>0</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>247</v>
@@ -25191,12 +25207,12 @@
       <c r="AQ61" s="15"/>
       <c r="AR61" s="15"/>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="15" t="s">
         <v>385</v>
       </c>
-      <c r="B62" s="39" t="s">
-        <v>246</v>
+      <c r="B62" s="75" t="n">
+        <v>0</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>247</v>
@@ -25299,12 +25315,12 @@
       <c r="AQ62" s="15"/>
       <c r="AR62" s="15"/>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="15" t="s">
         <v>390</v>
       </c>
-      <c r="B63" s="39" t="s">
-        <v>246</v>
+      <c r="B63" s="75" t="n">
+        <v>0</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>247</v>
@@ -25407,12 +25423,12 @@
       <c r="AQ63" s="15"/>
       <c r="AR63" s="15"/>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="15" t="s">
         <v>396</v>
       </c>
-      <c r="B64" s="39" t="s">
-        <v>246</v>
+      <c r="B64" s="75" t="n">
+        <v>0</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>247</v>
@@ -25515,11 +25531,11 @@
       <c r="AQ64" s="15"/>
       <c r="AR64" s="15"/>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="19" t="s">
         <v>709</v>
       </c>
-      <c r="B65" s="43" t="n">
+      <c r="B65" s="77" t="n">
         <v>0</v>
       </c>
       <c r="C65" s="19" t="s">
@@ -25623,11 +25639,11 @@
       <c r="AQ65" s="19"/>
       <c r="AR65" s="19"/>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="19" t="s">
         <v>710</v>
       </c>
-      <c r="B66" s="43" t="n">
+      <c r="B66" s="77" t="n">
         <v>0</v>
       </c>
       <c r="C66" s="19" t="s">
@@ -25731,11 +25747,11 @@
       <c r="AQ66" s="19"/>
       <c r="AR66" s="19"/>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="19" t="s">
         <v>711</v>
       </c>
-      <c r="B67" s="43" t="n">
+      <c r="B67" s="77" t="n">
         <v>0</v>
       </c>
       <c r="C67" s="19" t="s">
@@ -25839,11 +25855,11 @@
       <c r="AQ67" s="19"/>
       <c r="AR67" s="19"/>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="19" t="s">
         <v>712</v>
       </c>
-      <c r="B68" s="43" t="n">
+      <c r="B68" s="77" t="n">
         <v>0</v>
       </c>
       <c r="C68" s="19" t="s">
@@ -25947,11 +25963,11 @@
       <c r="AQ68" s="19"/>
       <c r="AR68" s="19"/>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="19" t="s">
         <v>713</v>
       </c>
-      <c r="B69" s="43" t="n">
+      <c r="B69" s="77" t="n">
         <v>0</v>
       </c>
       <c r="C69" s="19" t="s">
@@ -26055,11 +26071,11 @@
       <c r="AQ69" s="19"/>
       <c r="AR69" s="19"/>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="19" t="s">
         <v>714</v>
       </c>
-      <c r="B70" s="43" t="n">
+      <c r="B70" s="77" t="n">
         <v>0</v>
       </c>
       <c r="C70" s="19" t="s">
@@ -26167,8 +26183,8 @@
       <c r="A71" s="15" t="s">
         <v>419</v>
       </c>
-      <c r="B71" s="15" t="s">
-        <v>34</v>
+      <c r="B71" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C71" s="15" t="s">
         <v>420</v>
@@ -26275,12 +26291,12 @@
       <c r="AQ71" s="15"/>
       <c r="AR71" s="15"/>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="18" t="s">
         <v>432</v>
       </c>
-      <c r="B72" s="18" t="s">
-        <v>246</v>
+      <c r="B72" s="42" t="n">
+        <v>0</v>
       </c>
       <c r="C72" s="18" t="s">
         <v>247</v>
@@ -26379,12 +26395,12 @@
       <c r="AQ72" s="11"/>
       <c r="AR72" s="11"/>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="20" t="s">
         <v>846</v>
       </c>
-      <c r="B73" s="20" t="s">
-        <v>246</v>
+      <c r="B73" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="C73" s="20" t="s">
         <v>247</v>
@@ -26483,12 +26499,12 @@
       <c r="AQ73" s="20"/>
       <c r="AR73" s="20"/>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="20" t="s">
         <v>849</v>
       </c>
-      <c r="B74" s="20" t="s">
-        <v>246</v>
+      <c r="B74" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="C74" s="20" t="s">
         <v>247</v>
@@ -26587,12 +26603,12 @@
       <c r="AQ74" s="20"/>
       <c r="AR74" s="20"/>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="20" t="s">
         <v>851</v>
       </c>
-      <c r="B75" s="20" t="s">
-        <v>246</v>
+      <c r="B75" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="C75" s="20" t="s">
         <v>247</v>
@@ -26691,12 +26707,12 @@
       <c r="AQ75" s="20"/>
       <c r="AR75" s="20"/>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="11" t="s">
         <v>452</v>
       </c>
-      <c r="B76" s="11" t="s">
-        <v>246</v>
+      <c r="B76" s="14" t="n">
+        <v>0</v>
       </c>
       <c r="C76" s="11" t="s">
         <v>247</v>
@@ -26801,12 +26817,12 @@
       <c r="AQ76" s="11"/>
       <c r="AR76" s="11"/>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="20" t="s">
         <v>460</v>
       </c>
-      <c r="B77" s="20" t="s">
-        <v>246</v>
+      <c r="B77" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="C77" s="20" t="s">
         <v>247</v>
@@ -26911,12 +26927,12 @@
       <c r="AQ77" s="20"/>
       <c r="AR77" s="20"/>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="47" t="s">
         <v>463</v>
       </c>
-      <c r="B78" s="47" t="s">
-        <v>246</v>
+      <c r="B78" s="51" t="n">
+        <v>0</v>
       </c>
       <c r="C78" s="47" t="s">
         <v>247</v>
@@ -26930,7 +26946,7 @@
       <c r="F78" s="49" t="s">
         <v>251</v>
       </c>
-      <c r="G78" s="74" t="s">
+      <c r="G78" s="78" t="s">
         <v>57</v>
       </c>
       <c r="H78" s="49" t="s">
@@ -27021,12 +27037,12 @@
       <c r="AQ78" s="47"/>
       <c r="AR78" s="47"/>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="20" t="s">
         <v>469</v>
       </c>
-      <c r="B79" s="20" t="s">
-        <v>246</v>
+      <c r="B79" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="C79" s="20" t="s">
         <v>247</v>
@@ -27135,8 +27151,8 @@
       <c r="A80" s="11" t="s">
         <v>853</v>
       </c>
-      <c r="B80" s="11" t="s">
-        <v>34</v>
+      <c r="B80" s="14" t="n">
+        <v>1</v>
       </c>
       <c r="C80" s="11" t="s">
         <v>35</v>
@@ -27239,8 +27255,8 @@
       <c r="A81" s="20" t="s">
         <v>855</v>
       </c>
-      <c r="B81" s="20" t="s">
-        <v>34</v>
+      <c r="B81" s="22" t="n">
+        <v>1</v>
       </c>
       <c r="C81" s="20" t="s">
         <v>35</v>
@@ -27343,8 +27359,8 @@
       <c r="A82" s="11" t="s">
         <v>857</v>
       </c>
-      <c r="B82" s="11" t="s">
-        <v>34</v>
+      <c r="B82" s="14" t="n">
+        <v>1</v>
       </c>
       <c r="C82" s="11" t="s">
         <v>35</v>
@@ -27447,8 +27463,8 @@
       <c r="A83" s="20" t="s">
         <v>859</v>
       </c>
-      <c r="B83" s="20" t="s">
-        <v>34</v>
+      <c r="B83" s="22" t="n">
+        <v>1</v>
       </c>
       <c r="C83" s="20" t="s">
         <v>35</v>
@@ -27551,8 +27567,8 @@
       <c r="A84" s="11" t="s">
         <v>861</v>
       </c>
-      <c r="B84" s="11" t="s">
-        <v>34</v>
+      <c r="B84" s="14" t="n">
+        <v>1</v>
       </c>
       <c r="C84" s="11" t="s">
         <v>35</v>
@@ -27651,12 +27667,12 @@
       <c r="AQ84" s="11"/>
       <c r="AR84" s="11"/>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B85" s="47" t="s">
-        <v>246</v>
+      <c r="B85" s="51" t="n">
+        <v>0</v>
       </c>
       <c r="C85" s="47" t="s">
         <v>66</v>
@@ -27757,12 +27773,12 @@
       <c r="AQ85" s="47"/>
       <c r="AR85" s="47"/>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B86" s="47" t="s">
-        <v>246</v>
+      <c r="B86" s="51" t="n">
+        <v>0</v>
       </c>
       <c r="C86" s="47" t="s">
         <v>66</v>
@@ -27863,12 +27879,12 @@
       <c r="AQ86" s="47"/>
       <c r="AR86" s="47"/>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B87" s="47" t="s">
-        <v>246</v>
+      <c r="B87" s="51" t="n">
+        <v>0</v>
       </c>
       <c r="C87" s="47" t="s">
         <v>66</v>
@@ -27969,12 +27985,12 @@
       <c r="AQ87" s="47"/>
       <c r="AR87" s="47"/>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B88" s="47" t="s">
-        <v>246</v>
+      <c r="B88" s="51" t="n">
+        <v>0</v>
       </c>
       <c r="C88" s="47" t="s">
         <v>66</v>
@@ -28075,12 +28091,12 @@
       <c r="AQ88" s="47"/>
       <c r="AR88" s="47"/>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B89" s="47" t="s">
-        <v>246</v>
+      <c r="B89" s="51" t="n">
+        <v>0</v>
       </c>
       <c r="C89" s="47" t="s">
         <v>66</v>
@@ -28181,12 +28197,12 @@
       <c r="AQ89" s="47"/>
       <c r="AR89" s="47"/>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B90" s="47" t="s">
-        <v>246</v>
+      <c r="B90" s="51" t="n">
+        <v>0</v>
       </c>
       <c r="C90" s="47" t="s">
         <v>66</v>
@@ -28291,8 +28307,8 @@
       <c r="A91" s="15" t="s">
         <v>518</v>
       </c>
-      <c r="B91" s="15" t="s">
-        <v>34</v>
+      <c r="B91" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C91" s="15" t="s">
         <v>35</v>
@@ -28395,8 +28411,8 @@
       <c r="A92" s="15" t="s">
         <v>531</v>
       </c>
-      <c r="B92" s="15" t="s">
-        <v>34</v>
+      <c r="B92" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C92" s="15" t="s">
         <v>35</v>
@@ -28499,8 +28515,8 @@
       <c r="A93" s="15" t="s">
         <v>865</v>
       </c>
-      <c r="B93" s="15" t="s">
-        <v>34</v>
+      <c r="B93" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C93" s="15" t="s">
         <v>35</v>
@@ -28603,8 +28619,8 @@
       <c r="A94" s="20" t="s">
         <v>543</v>
       </c>
-      <c r="B94" s="20" t="s">
-        <v>34</v>
+      <c r="B94" s="22" t="n">
+        <v>1</v>
       </c>
       <c r="C94" s="20" t="s">
         <v>35</v>
@@ -28707,8 +28723,8 @@
       <c r="A95" s="15" t="s">
         <v>546</v>
       </c>
-      <c r="B95" s="15" t="s">
-        <v>34</v>
+      <c r="B95" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C95" s="15" t="s">
         <v>35</v>
@@ -28811,8 +28827,8 @@
       <c r="A96" s="15" t="s">
         <v>555</v>
       </c>
-      <c r="B96" s="15" t="s">
-        <v>34</v>
+      <c r="B96" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C96" s="15" t="s">
         <v>35</v>
@@ -28915,8 +28931,8 @@
       <c r="A97" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="B97" s="15" t="s">
-        <v>34</v>
+      <c r="B97" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C97" s="15" t="s">
         <v>35</v>
@@ -29019,8 +29035,8 @@
       <c r="A98" s="15" t="s">
         <v>574</v>
       </c>
-      <c r="B98" s="15" t="s">
-        <v>34</v>
+      <c r="B98" s="17" t="n">
+        <v>1</v>
       </c>
       <c r="C98" s="15" t="s">
         <v>35</v>
@@ -29119,12 +29135,12 @@
       <c r="AQ98" s="15"/>
       <c r="AR98" s="15"/>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="15" t="s">
         <v>582</v>
       </c>
-      <c r="B99" s="39" t="s">
-        <v>246</v>
+      <c r="B99" s="75" t="n">
+        <v>0</v>
       </c>
       <c r="C99" s="15"/>
       <c r="D99" s="16" t="n">
@@ -29229,12 +29245,12 @@
       <c r="AQ99" s="15"/>
       <c r="AR99" s="15"/>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="15" t="s">
         <v>591</v>
       </c>
-      <c r="B100" s="39" t="s">
-        <v>246</v>
+      <c r="B100" s="75" t="n">
+        <v>0</v>
       </c>
       <c r="C100" s="15"/>
       <c r="D100" s="16" t="n">
@@ -29339,12 +29355,12 @@
       <c r="AQ100" s="15"/>
       <c r="AR100" s="15"/>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="20" t="s">
         <v>876</v>
       </c>
-      <c r="B101" s="55" t="s">
-        <v>246</v>
+      <c r="B101" s="77" t="n">
+        <v>0</v>
       </c>
       <c r="C101" s="20"/>
       <c r="D101" s="19" t="n">
@@ -29449,12 +29465,12 @@
       <c r="AQ101" s="20"/>
       <c r="AR101" s="20"/>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="11" t="s">
         <v>600</v>
       </c>
-      <c r="B102" s="40" t="s">
-        <v>246</v>
+      <c r="B102" s="76" t="n">
+        <v>0</v>
       </c>
       <c r="C102" s="11"/>
       <c r="D102" s="12" t="n">
@@ -29559,12 +29575,12 @@
       <c r="AQ102" s="11"/>
       <c r="AR102" s="11"/>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="11" t="s">
         <v>604</v>
       </c>
-      <c r="B103" s="40" t="s">
-        <v>246</v>
+      <c r="B103" s="76" t="n">
+        <v>0</v>
       </c>
       <c r="C103" s="11"/>
       <c r="D103" s="12" t="n">
@@ -29669,12 +29685,12 @@
       <c r="AQ103" s="11"/>
       <c r="AR103" s="11"/>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="20" t="s">
         <v>878</v>
       </c>
-      <c r="B104" s="55" t="s">
-        <v>246</v>
+      <c r="B104" s="77" t="n">
+        <v>0</v>
       </c>
       <c r="C104" s="20"/>
       <c r="D104" s="19" t="n">
@@ -29779,12 +29795,12 @@
       <c r="AQ104" s="20"/>
       <c r="AR104" s="20"/>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="15" t="s">
         <v>609</v>
       </c>
-      <c r="B105" s="15" t="s">
-        <v>246</v>
+      <c r="B105" s="17" t="n">
+        <v>0</v>
       </c>
       <c r="C105" s="15"/>
       <c r="D105" s="16" t="n">
@@ -29889,12 +29905,12 @@
       <c r="AQ105" s="15"/>
       <c r="AR105" s="15"/>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="15" t="s">
         <v>617</v>
       </c>
-      <c r="B106" s="15" t="s">
-        <v>246</v>
+      <c r="B106" s="17" t="n">
+        <v>0</v>
       </c>
       <c r="C106" s="15"/>
       <c r="D106" s="16" t="n">
@@ -29999,12 +30015,12 @@
       <c r="AQ106" s="15"/>
       <c r="AR106" s="15"/>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="11" t="s">
         <v>879</v>
       </c>
-      <c r="B107" s="11" t="s">
-        <v>246</v>
+      <c r="B107" s="14" t="n">
+        <v>0</v>
       </c>
       <c r="C107" s="11"/>
       <c r="D107" s="12" t="n">
@@ -30109,12 +30125,12 @@
       <c r="AQ107" s="11"/>
       <c r="AR107" s="11"/>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B108" s="47" t="s">
-        <v>246</v>
+      <c r="B108" s="51" t="n">
+        <v>0</v>
       </c>
       <c r="C108" s="47"/>
       <c r="D108" s="48" t="n">
@@ -30213,12 +30229,12 @@
       <c r="AQ108" s="47"/>
       <c r="AR108" s="47"/>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B109" s="47" t="s">
-        <v>246</v>
+      <c r="B109" s="51" t="n">
+        <v>0</v>
       </c>
       <c r="C109" s="47"/>
       <c r="D109" s="48" t="n">
@@ -30317,12 +30333,12 @@
       <c r="AQ109" s="47"/>
       <c r="AR109" s="47"/>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="36" t="s">
         <v>634</v>
       </c>
-      <c r="B110" s="36" t="s">
-        <v>246</v>
+      <c r="B110" s="53" t="n">
+        <v>0</v>
       </c>
       <c r="C110" s="36"/>
       <c r="D110" s="59" t="n">
@@ -30421,12 +30437,12 @@
       <c r="AQ110" s="60"/>
       <c r="AR110" s="60"/>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="20" t="s">
         <v>638</v>
       </c>
-      <c r="B111" s="20" t="s">
-        <v>246</v>
+      <c r="B111" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="C111" s="20"/>
       <c r="D111" s="59" t="n">
@@ -30523,11 +30539,11 @@
       <c r="AQ111" s="60"/>
       <c r="AR111" s="60"/>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="19" t="s">
         <v>714</v>
       </c>
-      <c r="B112" s="19" t="n">
+      <c r="B112" s="22" t="n">
         <v>0</v>
       </c>
       <c r="C112" s="19"/>
@@ -30625,12 +30641,12 @@
       <c r="AQ112" s="60"/>
       <c r="AR112" s="60"/>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B113" s="60" t="s">
-        <v>246</v>
+      <c r="B113" s="61" t="n">
+        <v>0</v>
       </c>
       <c r="C113" s="60"/>
       <c r="D113" s="59" t="n">
@@ -30727,12 +30743,12 @@
       <c r="AQ113" s="60"/>
       <c r="AR113" s="60"/>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B114" s="60" t="s">
-        <v>246</v>
+      <c r="B114" s="61" t="n">
+        <v>0</v>
       </c>
       <c r="C114" s="60"/>
       <c r="D114" s="59" t="n">
@@ -30829,12 +30845,12 @@
       <c r="AQ114" s="60"/>
       <c r="AR114" s="60"/>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B115" s="60" t="s">
-        <v>246</v>
+      <c r="B115" s="61" t="n">
+        <v>0</v>
       </c>
       <c r="C115" s="60"/>
       <c r="D115" s="59" t="n">
@@ -30931,12 +30947,12 @@
       <c r="AQ115" s="60"/>
       <c r="AR115" s="60"/>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B116" s="60" t="s">
-        <v>246</v>
+      <c r="B116" s="61" t="n">
+        <v>0</v>
       </c>
       <c r="C116" s="60"/>
       <c r="D116" s="59" t="n">
@@ -31033,12 +31049,12 @@
       <c r="AQ116" s="60"/>
       <c r="AR116" s="60"/>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B117" s="60" t="s">
-        <v>246</v>
+      <c r="B117" s="61" t="n">
+        <v>0</v>
       </c>
       <c r="C117" s="60"/>
       <c r="D117" s="59" t="n">
@@ -31135,12 +31151,12 @@
       <c r="AQ117" s="60"/>
       <c r="AR117" s="60"/>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B118" s="60" t="s">
-        <v>246</v>
+      <c r="B118" s="61" t="n">
+        <v>0</v>
       </c>
       <c r="C118" s="60"/>
       <c r="D118" s="59" t="n">
@@ -31237,12 +31253,12 @@
       <c r="AQ118" s="60"/>
       <c r="AR118" s="60"/>
     </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="20" t="s">
         <v>662</v>
       </c>
-      <c r="B119" s="20" t="s">
-        <v>246</v>
+      <c r="B119" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="C119" s="20"/>
       <c r="D119" s="59" t="n">
@@ -31339,12 +31355,12 @@
       <c r="AQ119" s="60"/>
       <c r="AR119" s="60"/>
     </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="20" t="s">
         <v>665</v>
       </c>
-      <c r="B120" s="20" t="s">
-        <v>246</v>
+      <c r="B120" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="C120" s="20"/>
       <c r="D120" s="59" t="n">
@@ -31441,12 +31457,12 @@
       <c r="AQ120" s="60"/>
       <c r="AR120" s="60"/>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B121" s="60" t="s">
-        <v>246</v>
+      <c r="B121" s="61" t="n">
+        <v>0</v>
       </c>
       <c r="C121" s="60"/>
       <c r="D121" s="59" t="n">
@@ -31543,12 +31559,12 @@
       <c r="AQ121" s="60"/>
       <c r="AR121" s="60"/>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="33" t="s">
         <v>543</v>
       </c>
-      <c r="B122" s="33" t="s">
-        <v>246</v>
+      <c r="B122" s="74" t="n">
+        <v>0</v>
       </c>
       <c r="C122" s="33"/>
       <c r="D122" s="59" t="n">
@@ -31645,12 +31661,12 @@
       <c r="AQ122" s="60"/>
       <c r="AR122" s="60"/>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="20" t="s">
         <v>878</v>
       </c>
-      <c r="B123" s="20" t="s">
-        <v>246</v>
+      <c r="B123" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="C123" s="20"/>
       <c r="D123" s="59" t="n">
@@ -31747,12 +31763,12 @@
       <c r="AQ123" s="60"/>
       <c r="AR123" s="60"/>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="20" t="s">
         <v>876</v>
       </c>
-      <c r="B124" s="20" t="s">
-        <v>246</v>
+      <c r="B124" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="C124" s="20"/>
       <c r="D124" s="59" t="n">
@@ -31849,12 +31865,12 @@
       <c r="AQ124" s="60"/>
       <c r="AR124" s="60"/>
     </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B125" s="60" t="s">
-        <v>246</v>
+      <c r="B125" s="61" t="n">
+        <v>0</v>
       </c>
       <c r="C125" s="60"/>
       <c r="D125" s="59" t="n">
@@ -31951,12 +31967,12 @@
       <c r="AQ125" s="60"/>
       <c r="AR125" s="60"/>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B126" s="60" t="s">
-        <v>246</v>
+      <c r="B126" s="61" t="n">
+        <v>0</v>
       </c>
       <c r="C126" s="60"/>
       <c r="D126" s="59" t="n">
@@ -32054,13 +32070,7 @@
       <c r="AR126" s="60"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH126">
-    <filterColumn colId="1">
-      <customFilters and="true">
-        <customFilter operator="equal" val="1"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AH126"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -32080,509 +32090,509 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="1" sqref="15:36 F11"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="75" width="4.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="75" width="33.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="75" width="27.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="75" width="60.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="75" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="76" width="82.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="75" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="79" width="4.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="79" width="33.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="79" width="27.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="79" width="60.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="79" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="80" width="82.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="79" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="122.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="81" t="s">
         <v>882</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="82" t="s">
         <v>883</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="82" t="s">
         <v>884</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="82" t="s">
         <v>885</v>
       </c>
-      <c r="E2" s="78" t="s">
+      <c r="E2" s="82" t="s">
         <v>886</v>
       </c>
-      <c r="F2" s="79" t="s">
+      <c r="F2" s="83" t="s">
         <v>887</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="79" t="s">
         <v>888</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80" t="s">
+      <c r="C3" s="84"/>
+      <c r="D3" s="84" t="s">
         <v>889</v>
       </c>
-      <c r="E3" s="80" t="s">
+      <c r="E3" s="84" t="s">
         <v>890</v>
       </c>
-      <c r="F3" s="81" t="s">
+      <c r="F3" s="85" t="s">
         <v>891</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="79" t="s">
         <v>892</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80" t="s">
+      <c r="C4" s="84"/>
+      <c r="D4" s="84" t="s">
         <v>893</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="81" t="s">
+      <c r="E4" s="84"/>
+      <c r="F4" s="85" t="s">
         <v>894</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="79" t="s">
         <v>895</v>
       </c>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="84" t="s">
         <v>896</v>
       </c>
-      <c r="C5" s="80"/>
-      <c r="D5" s="82" t="s">
+      <c r="C5" s="84"/>
+      <c r="D5" s="86" t="s">
         <v>897</v>
       </c>
-      <c r="E5" s="80" t="s">
+      <c r="E5" s="84" t="s">
         <v>898</v>
       </c>
-      <c r="F5" s="83" t="s">
+      <c r="F5" s="87" t="s">
         <v>899</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="79" t="s">
         <v>900</v>
       </c>
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80" t="s">
+      <c r="C6" s="84"/>
+      <c r="D6" s="84" t="s">
         <v>893</v>
       </c>
-      <c r="E6" s="80"/>
-      <c r="F6" s="81" t="s">
+      <c r="E6" s="84"/>
+      <c r="F6" s="85" t="s">
         <v>901</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="79" t="s">
         <v>902</v>
       </c>
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80" t="s">
+      <c r="C7" s="84"/>
+      <c r="D7" s="84" t="s">
         <v>893</v>
       </c>
-      <c r="E7" s="80"/>
-      <c r="F7" s="81"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="85"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="79" t="s">
         <v>903</v>
       </c>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="84" t="s">
         <v>904</v>
       </c>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80" t="s">
+      <c r="C8" s="84"/>
+      <c r="D8" s="84" t="s">
         <v>893</v>
       </c>
-      <c r="E8" s="80"/>
-      <c r="F8" s="81"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="85"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="79" t="s">
         <v>905</v>
       </c>
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80" t="s">
+      <c r="C9" s="84"/>
+      <c r="D9" s="84" t="s">
         <v>893</v>
       </c>
-      <c r="E9" s="80"/>
-      <c r="F9" s="81"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="85"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="79" t="s">
         <v>906</v>
       </c>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="84" t="s">
         <v>907</v>
       </c>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80" t="s">
+      <c r="C10" s="84"/>
+      <c r="D10" s="84" t="s">
         <v>908</v>
       </c>
-      <c r="E10" s="80"/>
-      <c r="F10" s="81" t="s">
+      <c r="E10" s="84"/>
+      <c r="F10" s="85" t="s">
         <v>909</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="79" t="s">
         <v>910</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80" t="s">
+      <c r="C11" s="84"/>
+      <c r="D11" s="84" t="s">
         <v>911</v>
       </c>
-      <c r="E11" s="80"/>
-      <c r="F11" s="81" t="s">
+      <c r="E11" s="84"/>
+      <c r="F11" s="85" t="s">
         <v>909</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="79" t="s">
         <v>912</v>
       </c>
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="84" t="s">
         <v>913</v>
       </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80" t="s">
+      <c r="C12" s="84"/>
+      <c r="D12" s="84" t="s">
         <v>914</v>
       </c>
-      <c r="E12" s="80"/>
-      <c r="F12" s="81"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="85"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="75" t="s">
+      <c r="A13" s="79" t="s">
         <v>915</v>
       </c>
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="80" t="s">
+      <c r="C13" s="84" t="s">
         <v>916</v>
       </c>
-      <c r="D13" s="82" t="s">
+      <c r="D13" s="86" t="s">
         <v>917</v>
       </c>
-      <c r="E13" s="80" t="s">
+      <c r="E13" s="84" t="s">
         <v>918</v>
       </c>
-      <c r="F13" s="83" t="s">
+      <c r="F13" s="87" t="s">
         <v>899</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="75" t="s">
+      <c r="A14" s="79" t="s">
         <v>919</v>
       </c>
-      <c r="B14" s="84" t="s">
+      <c r="B14" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="80"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="83"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="84"/>
+      <c r="F14" s="87"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="75" t="s">
+      <c r="A15" s="79" t="s">
         <v>920</v>
       </c>
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80" t="s">
+      <c r="C15" s="84"/>
+      <c r="D15" s="84" t="s">
         <v>921</v>
       </c>
-      <c r="E15" s="80"/>
-      <c r="F15" s="83" t="s">
+      <c r="E15" s="84"/>
+      <c r="F15" s="87" t="s">
         <v>922</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="75" t="s">
+      <c r="A16" s="79" t="s">
         <v>923</v>
       </c>
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="80"/>
-      <c r="D16" s="82" t="s">
+      <c r="C16" s="84"/>
+      <c r="D16" s="86" t="s">
         <v>924</v>
       </c>
-      <c r="E16" s="80"/>
-      <c r="F16" s="83" t="s">
+      <c r="E16" s="84"/>
+      <c r="F16" s="87" t="s">
         <v>899</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="75" t="s">
+      <c r="A17" s="79" t="s">
         <v>925</v>
       </c>
-      <c r="B17" s="80" t="s">
+      <c r="B17" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="80"/>
-      <c r="D17" s="82" t="s">
+      <c r="C17" s="84"/>
+      <c r="D17" s="86" t="s">
         <v>926</v>
       </c>
-      <c r="E17" s="80"/>
-      <c r="F17" s="83" t="s">
+      <c r="E17" s="84"/>
+      <c r="F17" s="87" t="s">
         <v>899</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="75" t="s">
+      <c r="A18" s="79" t="s">
         <v>927</v>
       </c>
-      <c r="B18" s="80" t="s">
+      <c r="B18" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="80"/>
-      <c r="D18" s="80" t="s">
+      <c r="C18" s="84"/>
+      <c r="D18" s="84" t="s">
         <v>928</v>
       </c>
-      <c r="E18" s="80"/>
-      <c r="F18" s="81" t="s">
+      <c r="E18" s="84"/>
+      <c r="F18" s="85" t="s">
         <v>929</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="75" t="s">
+      <c r="A19" s="79" t="s">
         <v>930</v>
       </c>
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="82" t="s">
+      <c r="C19" s="84"/>
+      <c r="D19" s="86" t="s">
         <v>931</v>
       </c>
-      <c r="E19" s="80"/>
-      <c r="F19" s="83" t="s">
+      <c r="E19" s="84"/>
+      <c r="F19" s="87" t="s">
         <v>932</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="75" t="s">
+      <c r="A20" s="79" t="s">
         <v>933</v>
       </c>
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80" t="s">
+      <c r="C20" s="84"/>
+      <c r="D20" s="84" t="s">
         <v>934</v>
       </c>
-      <c r="E20" s="80"/>
-      <c r="F20" s="81" t="s">
+      <c r="E20" s="84"/>
+      <c r="F20" s="85" t="s">
         <v>935</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="79" t="s">
         <v>936</v>
       </c>
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="80"/>
-      <c r="D21" s="82" t="s">
+      <c r="C21" s="84"/>
+      <c r="D21" s="86" t="s">
         <v>937</v>
       </c>
-      <c r="E21" s="80"/>
-      <c r="F21" s="81" t="s">
+      <c r="E21" s="84"/>
+      <c r="F21" s="85" t="s">
         <v>938</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="79" t="s">
         <v>939</v>
       </c>
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="85" t="s">
+      <c r="C22" s="89" t="s">
         <v>940</v>
       </c>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80" t="s">
+      <c r="D22" s="84"/>
+      <c r="E22" s="84" t="s">
         <v>890</v>
       </c>
-      <c r="F22" s="81" t="s">
+      <c r="F22" s="85" t="s">
         <v>941</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="75" t="s">
+      <c r="A23" s="79" t="s">
         <v>942</v>
       </c>
-      <c r="B23" s="80" t="s">
+      <c r="B23" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="85"/>
-      <c r="D23" s="82" t="s">
+      <c r="C23" s="89"/>
+      <c r="D23" s="86" t="s">
         <v>931</v>
       </c>
-      <c r="E23" s="80" t="s">
+      <c r="E23" s="84" t="s">
         <v>918</v>
       </c>
-      <c r="F23" s="83" t="s">
+      <c r="F23" s="87" t="s">
         <v>943</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="75" t="s">
+      <c r="A24" s="79" t="s">
         <v>944</v>
       </c>
-      <c r="B24" s="80" t="s">
+      <c r="B24" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="85"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80" t="s">
+      <c r="C24" s="89"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="84" t="s">
         <v>945</v>
       </c>
-      <c r="F24" s="83" t="s">
+      <c r="F24" s="87" t="s">
         <v>946</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="86" t="s">
+      <c r="A25" s="90" t="s">
         <v>947</v>
       </c>
-      <c r="B25" s="80" t="s">
+      <c r="B25" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="85"/>
-      <c r="D25" s="82" t="s">
+      <c r="C25" s="89"/>
+      <c r="D25" s="86" t="s">
         <v>931</v>
       </c>
-      <c r="E25" s="80" t="s">
+      <c r="E25" s="84" t="s">
         <v>918</v>
       </c>
-      <c r="F25" s="83" t="s">
+      <c r="F25" s="87" t="s">
         <v>948</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="75" t="s">
+      <c r="A26" s="79" t="s">
         <v>949</v>
       </c>
-      <c r="B26" s="80" t="s">
+      <c r="B26" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="85"/>
-      <c r="D26" s="80" t="s">
+      <c r="C26" s="89"/>
+      <c r="D26" s="84" t="s">
         <v>893</v>
       </c>
-      <c r="E26" s="80"/>
-      <c r="F26" s="81"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="85"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="75" t="s">
+      <c r="A27" s="79" t="s">
         <v>950</v>
       </c>
-      <c r="B27" s="80" t="s">
+      <c r="B27" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="85" t="s">
+      <c r="C27" s="89" t="s">
         <v>951</v>
       </c>
-      <c r="D27" s="80" t="s">
+      <c r="D27" s="84" t="s">
         <v>952</v>
       </c>
-      <c r="E27" s="81" t="s">
+      <c r="E27" s="85" t="s">
         <v>953</v>
       </c>
-      <c r="F27" s="81" t="s">
+      <c r="F27" s="85" t="s">
         <v>909</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="75" t="s">
+      <c r="A28" s="79" t="s">
         <v>954</v>
       </c>
-      <c r="B28" s="80" t="s">
+      <c r="B28" s="84" t="s">
         <v>955</v>
       </c>
-      <c r="C28" s="85"/>
-      <c r="D28" s="80" t="s">
+      <c r="C28" s="89"/>
+      <c r="D28" s="84" t="s">
         <v>956</v>
       </c>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81" t="s">
+      <c r="E28" s="85"/>
+      <c r="F28" s="85" t="s">
         <v>957</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="75" t="s">
+      <c r="A29" s="79" t="s">
         <v>958</v>
       </c>
-      <c r="B29" s="80" t="s">
+      <c r="B29" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="85"/>
-      <c r="D29" s="80"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="81" t="s">
+      <c r="C29" s="89"/>
+      <c r="D29" s="84"/>
+      <c r="E29" s="85"/>
+      <c r="F29" s="85" t="s">
         <v>909</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="75" t="s">
+      <c r="A30" s="79" t="s">
         <v>959</v>
       </c>
-      <c r="B30" s="80" t="s">
+      <c r="B30" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="85"/>
-      <c r="D30" s="80"/>
-      <c r="E30" s="81"/>
-      <c r="F30" s="81" t="s">
+      <c r="C30" s="89"/>
+      <c r="D30" s="84"/>
+      <c r="E30" s="85"/>
+      <c r="F30" s="85" t="s">
         <v>909</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="75" t="s">
+      <c r="A31" s="79" t="s">
         <v>960</v>
       </c>
-      <c r="B31" s="80" t="s">
+      <c r="B31" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="80"/>
-      <c r="D31" s="80" t="s">
+      <c r="C31" s="84"/>
+      <c r="D31" s="84" t="s">
         <v>961</v>
       </c>
-      <c r="E31" s="80" t="s">
+      <c r="E31" s="84" t="s">
         <v>962</v>
       </c>
-      <c r="F31" s="85" t="s">
+      <c r="F31" s="89" t="s">
         <v>963</v>
       </c>
     </row>
@@ -32590,13 +32600,13 @@
       <c r="A32" s="0" t="s">
         <v>964</v>
       </c>
-      <c r="B32" s="80" t="s">
+      <c r="B32" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="80"/>
-      <c r="D32" s="80"/>
-      <c r="E32" s="80"/>
-      <c r="F32" s="85" t="s">
+      <c r="C32" s="84"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="89" t="s">
         <v>963</v>
       </c>
     </row>
@@ -32604,13 +32614,13 @@
       <c r="A33" s="0" t="s">
         <v>965</v>
       </c>
-      <c r="B33" s="80" t="s">
+      <c r="B33" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="80"/>
-      <c r="D33" s="80"/>
-      <c r="E33" s="80"/>
-      <c r="F33" s="85" t="s">
+      <c r="C33" s="84"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="89" t="s">
         <v>963</v>
       </c>
     </row>
@@ -32618,13 +32628,13 @@
       <c r="A34" s="0" t="s">
         <v>966</v>
       </c>
-      <c r="B34" s="80" t="s">
+      <c r="B34" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="80"/>
-      <c r="D34" s="80"/>
-      <c r="E34" s="80"/>
-      <c r="F34" s="85" t="s">
+      <c r="C34" s="84"/>
+      <c r="D34" s="84"/>
+      <c r="E34" s="84"/>
+      <c r="F34" s="89" t="s">
         <v>963</v>
       </c>
     </row>
@@ -32658,7 +32668,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="15:36"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32672,27 +32682,27 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>967</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="91" t="s">
         <v>968</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="91" t="s">
         <v>969</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="91" t="s">
         <v>970</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="91" t="s">
         <v>971</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="90" t="s">
         <v>972</v>
       </c>
-      <c r="B2" s="86" t="n">
+      <c r="B2" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -32703,10 +32713,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="90" t="s">
         <v>975</v>
       </c>
-      <c r="B3" s="86" t="n">
+      <c r="B3" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -32717,10 +32727,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="90" t="s">
         <v>977</v>
       </c>
-      <c r="B4" s="86" t="n">
+      <c r="B4" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -32731,10 +32741,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="90" t="s">
         <v>979</v>
       </c>
-      <c r="B5" s="86" t="n">
+      <c r="B5" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
@@ -32745,10 +32755,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="90" t="s">
         <v>981</v>
       </c>
-      <c r="B6" s="86" t="n">
+      <c r="B6" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
@@ -32759,10 +32769,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="86" t="s">
+      <c r="A7" s="90" t="s">
         <v>983</v>
       </c>
-      <c r="B7" s="86" t="n">
+      <c r="B7" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C7" s="0" t="s">
@@ -32773,10 +32783,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="86" t="s">
+      <c r="A8" s="90" t="s">
         <v>985</v>
       </c>
-      <c r="B8" s="86" t="n">
+      <c r="B8" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
@@ -32787,27 +32797,27 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="90" t="s">
         <v>987</v>
       </c>
-      <c r="B9" s="86" t="n">
+      <c r="B9" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>988</v>
       </c>
-      <c r="D9" s="88" t="s">
+      <c r="D9" s="92" t="s">
         <v>989</v>
       </c>
-      <c r="E9" s="88" t="s">
+      <c r="E9" s="92" t="s">
         <v>990</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="86" t="s">
+      <c r="A10" s="90" t="s">
         <v>991</v>
       </c>
-      <c r="B10" s="86" t="n">
+      <c r="B10" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C10" s="0" t="s">
@@ -32818,10 +32828,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="86" t="s">
+      <c r="A11" s="90" t="s">
         <v>993</v>
       </c>
-      <c r="B11" s="86" t="n">
+      <c r="B11" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C11" s="0" t="s">
@@ -32832,10 +32842,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="86" t="s">
+      <c r="A12" s="90" t="s">
         <v>995</v>
       </c>
-      <c r="B12" s="86" t="n">
+      <c r="B12" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C12" s="0" t="s">
@@ -32846,10 +32856,10 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="86" t="s">
+      <c r="A13" s="90" t="s">
         <v>997</v>
       </c>
-      <c r="B13" s="86" t="n">
+      <c r="B13" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C13" s="0" t="s">
@@ -32860,10 +32870,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="86" t="s">
+      <c r="A14" s="90" t="s">
         <v>999</v>
       </c>
-      <c r="B14" s="86" t="n">
+      <c r="B14" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C14" s="0" t="s">
@@ -32874,10 +32884,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="86" t="s">
+      <c r="A15" s="90" t="s">
         <v>1001</v>
       </c>
-      <c r="B15" s="86" t="n">
+      <c r="B15" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C15" s="0" t="s">
@@ -32886,15 +32896,15 @@
       <c r="D15" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="89" t="s">
+      <c r="E15" s="93" t="s">
         <v>1003</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="86" t="s">
+      <c r="A16" s="90" t="s">
         <v>1004</v>
       </c>
-      <c r="B16" s="86" t="n">
+      <c r="B16" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C16" s="0" t="s">
@@ -32903,13 +32913,13 @@
       <c r="D16" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="89"/>
+      <c r="E16" s="93"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="86" t="s">
+      <c r="A17" s="90" t="s">
         <v>1006</v>
       </c>
-      <c r="B17" s="86" t="n">
+      <c r="B17" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C17" s="0" t="s">
@@ -32918,13 +32928,13 @@
       <c r="D17" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="89"/>
+      <c r="E17" s="93"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="86" t="s">
+      <c r="A18" s="90" t="s">
         <v>1008</v>
       </c>
-      <c r="B18" s="86" t="n">
+      <c r="B18" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C18" s="0" t="s">
@@ -32933,13 +32943,13 @@
       <c r="D18" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="89"/>
+      <c r="E18" s="93"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="86" t="s">
+      <c r="A19" s="90" t="s">
         <v>1010</v>
       </c>
-      <c r="B19" s="86" t="n">
+      <c r="B19" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C19" s="0" t="s">
@@ -32950,24 +32960,24 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="86" t="s">
+      <c r="A20" s="90" t="s">
         <v>1013</v>
       </c>
-      <c r="B20" s="86" t="n">
+      <c r="B20" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>1014</v>
       </c>
-      <c r="E20" s="89" t="s">
+      <c r="E20" s="93" t="s">
         <v>1015</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="86" t="s">
+      <c r="A21" s="90" t="s">
         <v>1016</v>
       </c>
-      <c r="B21" s="86" t="n">
+      <c r="B21" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C21" s="0" t="s">
@@ -32976,13 +32986,13 @@
       <c r="D21" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="89"/>
+      <c r="E21" s="93"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="86" t="s">
+      <c r="A22" s="90" t="s">
         <v>1018</v>
       </c>
-      <c r="B22" s="86" t="n">
+      <c r="B22" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C22" s="0" t="s">
@@ -32991,13 +33001,13 @@
       <c r="D22" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="89"/>
+      <c r="E22" s="93"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="86" t="s">
+      <c r="A23" s="90" t="s">
         <v>1020</v>
       </c>
-      <c r="B23" s="86" t="n">
+      <c r="B23" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C23" s="0" t="s">
@@ -33008,10 +33018,10 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="86" t="s">
+      <c r="A24" s="90" t="s">
         <v>1022</v>
       </c>
-      <c r="B24" s="86" t="n">
+      <c r="B24" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C24" s="0" t="s">
@@ -33019,10 +33029,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="86" t="s">
+      <c r="A25" s="90" t="s">
         <v>1024</v>
       </c>
-      <c r="B25" s="86" t="n">
+      <c r="B25" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C25" s="0" t="s">
@@ -33030,10 +33040,10 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="86" t="s">
+      <c r="A26" s="90" t="s">
         <v>1026</v>
       </c>
-      <c r="B26" s="86" t="n">
+      <c r="B26" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C26" s="0" t="s">
@@ -33044,10 +33054,10 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="86" t="s">
+      <c r="A27" s="90" t="s">
         <v>1029</v>
       </c>
-      <c r="B27" s="86" t="n">
+      <c r="B27" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C27" s="0" t="s">
@@ -33058,10 +33068,10 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="86" t="s">
+      <c r="A28" s="90" t="s">
         <v>1032</v>
       </c>
-      <c r="B28" s="86" t="n">
+      <c r="B28" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C28" s="0" t="s">
@@ -33072,10 +33082,10 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="86" t="s">
+      <c r="A29" s="90" t="s">
         <v>1034</v>
       </c>
-      <c r="B29" s="86" t="n">
+      <c r="B29" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C29" s="0" t="s">
@@ -33086,10 +33096,10 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="86" t="s">
+      <c r="A30" s="90" t="s">
         <v>1036</v>
       </c>
-      <c r="B30" s="86" t="n">
+      <c r="B30" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C30" s="0" t="s">
@@ -33100,10 +33110,10 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="86" t="s">
+      <c r="A31" s="90" t="s">
         <v>1038</v>
       </c>
-      <c r="B31" s="86" t="n">
+      <c r="B31" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C31" s="0" t="s">
@@ -33114,10 +33124,10 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="86" t="s">
+      <c r="A32" s="90" t="s">
         <v>1040</v>
       </c>
-      <c r="B32" s="86" t="n">
+      <c r="B32" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C32" s="0" t="s">
@@ -33128,10 +33138,10 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="86" t="s">
+      <c r="A33" s="90" t="s">
         <v>1042</v>
       </c>
-      <c r="B33" s="86" t="n">
+      <c r="B33" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C33" s="0" t="s">
@@ -33142,10 +33152,10 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="86" t="s">
+      <c r="A34" s="90" t="s">
         <v>1044</v>
       </c>
-      <c r="B34" s="86" t="n">
+      <c r="B34" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C34" s="0" t="s">
@@ -33156,10 +33166,10 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="86" t="s">
+      <c r="A35" s="90" t="s">
         <v>1046</v>
       </c>
-      <c r="B35" s="86" t="n">
+      <c r="B35" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C35" s="0" t="s">
@@ -33170,10 +33180,10 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="86" t="s">
+      <c r="A36" s="90" t="s">
         <v>1048</v>
       </c>
-      <c r="B36" s="86" t="n">
+      <c r="B36" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C36" s="0" t="s">
@@ -33184,10 +33194,10 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="86" t="s">
+      <c r="A37" s="90" t="s">
         <v>1050</v>
       </c>
-      <c r="B37" s="86" t="n">
+      <c r="B37" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C37" s="0" t="s">
@@ -33198,10 +33208,10 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="86" t="s">
+      <c r="A38" s="90" t="s">
         <v>1052</v>
       </c>
-      <c r="B38" s="86" t="n">
+      <c r="B38" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C38" s="0" t="s">
@@ -33212,10 +33222,10 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="86" t="s">
+      <c r="A39" s="90" t="s">
         <v>1054</v>
       </c>
-      <c r="B39" s="86" t="n">
+      <c r="B39" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C39" s="0" t="s">
@@ -33226,10 +33236,10 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="86" t="s">
+      <c r="A40" s="90" t="s">
         <v>1057</v>
       </c>
-      <c r="B40" s="86" t="n">
+      <c r="B40" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C40" s="0" t="s">
@@ -33240,10 +33250,10 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="86" t="s">
+      <c r="A41" s="90" t="s">
         <v>1058</v>
       </c>
-      <c r="B41" s="86" t="n">
+      <c r="B41" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C41" s="0" t="s">
@@ -33254,10 +33264,10 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="86" t="s">
+      <c r="A42" s="90" t="s">
         <v>1060</v>
       </c>
-      <c r="B42" s="86" t="n">
+      <c r="B42" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C42" s="0" t="s">
@@ -33268,10 +33278,10 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="86" t="s">
+      <c r="A43" s="90" t="s">
         <v>1063</v>
       </c>
-      <c r="B43" s="86" t="n">
+      <c r="B43" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C43" s="0" t="s">
@@ -33282,10 +33292,10 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="86" t="s">
+      <c r="A44" s="90" t="s">
         <v>1065</v>
       </c>
-      <c r="B44" s="86" t="n">
+      <c r="B44" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C44" s="0" t="s">
@@ -33296,10 +33306,10 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="86" t="s">
+      <c r="A45" s="90" t="s">
         <v>1067</v>
       </c>
-      <c r="B45" s="86" t="n">
+      <c r="B45" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C45" s="0" t="s">
@@ -33310,10 +33320,10 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="86" t="s">
+      <c r="A46" s="90" t="s">
         <v>1069</v>
       </c>
-      <c r="B46" s="86" t="n">
+      <c r="B46" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C46" s="0" t="s">
@@ -33324,10 +33334,10 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="86" t="s">
+      <c r="A47" s="90" t="s">
         <v>1071</v>
       </c>
-      <c r="B47" s="86" t="n">
+      <c r="B47" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C47" s="0" t="s">
@@ -33338,10 +33348,10 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="86" t="s">
+      <c r="A48" s="90" t="s">
         <v>1073</v>
       </c>
-      <c r="B48" s="86" t="n">
+      <c r="B48" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C48" s="0" t="s">
@@ -33352,10 +33362,10 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="86" t="s">
+      <c r="A49" s="90" t="s">
         <v>1075</v>
       </c>
-      <c r="B49" s="86" t="n">
+      <c r="B49" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C49" s="0" t="s">
@@ -33366,10 +33376,10 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="86" t="s">
+      <c r="A50" s="90" t="s">
         <v>1077</v>
       </c>
-      <c r="B50" s="86" t="n">
+      <c r="B50" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C50" s="0" t="s">
@@ -33380,10 +33390,10 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="86" t="s">
+      <c r="A51" s="90" t="s">
         <v>1079</v>
       </c>
-      <c r="B51" s="86" t="n">
+      <c r="B51" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C51" s="0" t="s">
@@ -33394,10 +33404,10 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="86" t="s">
+      <c r="A52" s="90" t="s">
         <v>1081</v>
       </c>
-      <c r="B52" s="86" t="n">
+      <c r="B52" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C52" s="0" t="s">
@@ -33408,10 +33418,10 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="86" t="s">
+      <c r="A53" s="90" t="s">
         <v>1083</v>
       </c>
-      <c r="B53" s="86" t="n">
+      <c r="B53" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C53" s="0" t="s">
@@ -33422,10 +33432,10 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="86" t="s">
+      <c r="A54" s="90" t="s">
         <v>1085</v>
       </c>
-      <c r="B54" s="86" t="n">
+      <c r="B54" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C54" s="0" t="s">
@@ -33436,10 +33446,10 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="86" t="s">
+      <c r="A55" s="90" t="s">
         <v>1088</v>
       </c>
-      <c r="B55" s="86" t="n">
+      <c r="B55" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C55" s="0" t="s">
@@ -33450,10 +33460,10 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="86" t="s">
+      <c r="A56" s="90" t="s">
         <v>1090</v>
       </c>
-      <c r="B56" s="86" t="n">
+      <c r="B56" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C56" s="0" t="s">
@@ -33464,10 +33474,10 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="86" t="s">
+      <c r="A57" s="90" t="s">
         <v>1092</v>
       </c>
-      <c r="B57" s="86" t="n">
+      <c r="B57" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C57" s="0" t="s">
@@ -33478,10 +33488,10 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="86" t="s">
+      <c r="A58" s="90" t="s">
         <v>1094</v>
       </c>
-      <c r="B58" s="86" t="n">
+      <c r="B58" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C58" s="0" t="s">
@@ -33492,10 +33502,10 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="86" t="s">
+      <c r="A59" s="90" t="s">
         <v>1097</v>
       </c>
-      <c r="B59" s="86" t="n">
+      <c r="B59" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C59" s="0" t="s">
@@ -33506,10 +33516,10 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="86" t="s">
+      <c r="A60" s="90" t="s">
         <v>1099</v>
       </c>
-      <c r="B60" s="86" t="n">
+      <c r="B60" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C60" s="0" t="s">
@@ -33520,10 +33530,10 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="86" t="s">
+      <c r="A61" s="90" t="s">
         <v>1101</v>
       </c>
-      <c r="B61" s="86" t="n">
+      <c r="B61" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C61" s="0" t="s">
@@ -33534,10 +33544,10 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="86" t="s">
+      <c r="A62" s="90" t="s">
         <v>1103</v>
       </c>
-      <c r="B62" s="86" t="n">
+      <c r="B62" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C62" s="0" t="s">
@@ -33548,10 +33558,10 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="86" t="s">
+      <c r="A63" s="90" t="s">
         <v>1105</v>
       </c>
-      <c r="B63" s="86" t="n">
+      <c r="B63" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C63" s="0" t="s">
@@ -33562,10 +33572,10 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="86" t="s">
+      <c r="A64" s="90" t="s">
         <v>1107</v>
       </c>
-      <c r="B64" s="86" t="n">
+      <c r="B64" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C64" s="0" t="s">
@@ -33576,10 +33586,10 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="86" t="s">
+      <c r="A65" s="90" t="s">
         <v>1109</v>
       </c>
-      <c r="B65" s="86" t="n">
+      <c r="B65" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C65" s="0" t="s">
@@ -33590,10 +33600,10 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="86" t="s">
+      <c r="A66" s="90" t="s">
         <v>1111</v>
       </c>
-      <c r="B66" s="86" t="n">
+      <c r="B66" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C66" s="0" t="s">
@@ -33604,10 +33614,10 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="86" t="s">
+      <c r="A67" s="90" t="s">
         <v>1114</v>
       </c>
-      <c r="B67" s="86" t="n">
+      <c r="B67" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C67" s="0" t="s">
@@ -33618,10 +33628,10 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="86" t="s">
+      <c r="A68" s="90" t="s">
         <v>1116</v>
       </c>
-      <c r="B68" s="86" t="n">
+      <c r="B68" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C68" s="0" t="s">
@@ -33632,10 +33642,10 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="86" t="s">
+      <c r="A69" s="90" t="s">
         <v>1118</v>
       </c>
-      <c r="B69" s="86" t="n">
+      <c r="B69" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C69" s="0" t="s">
@@ -33646,10 +33656,10 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="86" t="s">
+      <c r="A70" s="90" t="s">
         <v>1120</v>
       </c>
-      <c r="B70" s="86" t="n">
+      <c r="B70" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C70" s="0" t="s">
@@ -33660,10 +33670,10 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="86" t="s">
+      <c r="A71" s="90" t="s">
         <v>1122</v>
       </c>
-      <c r="B71" s="86" t="n">
+      <c r="B71" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C71" s="0" t="s">
@@ -33674,10 +33684,10 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="86" t="s">
+      <c r="A72" s="90" t="s">
         <v>1124</v>
       </c>
-      <c r="B72" s="86" t="n">
+      <c r="B72" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C72" s="0" t="s">
@@ -33688,10 +33698,10 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="86" t="s">
+      <c r="A73" s="90" t="s">
         <v>1126</v>
       </c>
-      <c r="B73" s="86" t="n">
+      <c r="B73" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C73" s="0" t="s">

</xml_diff>

<commit_message>
changed index function degreesum to temperaturesum
</commit_message>
<xml_diff>
--- a/climate_indices_CV22.xlsx
+++ b/climate_indices_CV22.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7708" uniqueCount="1128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7708" uniqueCount="1130">
   <si>
     <t xml:space="preserve">VarName</t>
   </si>
@@ -2626,6 +2626,9 @@
     <t xml:space="preserve">day_of_year</t>
   </si>
   <si>
+    <t xml:space="preserve">growing [temperaturesum]</t>
+  </si>
+  <si>
     <t xml:space="preserve">threshold, gsstart, gsend</t>
   </si>
   <si>
@@ -2699,6 +2702,9 @@
   </si>
   <si>
     <t xml:space="preserve">hddheat{TT}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temperaturesum</t>
   </si>
   <si>
     <t xml:space="preserve">Heating Degree Days (Tmean &lt; {TT}C)</t>
@@ -18746,7 +18752,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="bottomRight" activeCell="F110" activeCellId="0" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23099,13 +23105,13 @@
         <v>275</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>756</v>
+        <v>829</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>57</v>
       </c>
       <c r="H42" s="22" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="I42" s="22" t="n">
         <v>1</v>
@@ -23211,7 +23217,7 @@
         <v>281</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G43" s="29" t="n">
         <v>1</v>
@@ -23254,7 +23260,7 @@
         <v>46</v>
       </c>
       <c r="U43" s="8" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="V43" s="8"/>
       <c r="W43" s="8"/>
@@ -23316,7 +23322,7 @@
         <v>288</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G44" s="29" t="n">
         <v>1</v>
@@ -23359,7 +23365,7 @@
         <v>46</v>
       </c>
       <c r="U44" s="8" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="V44" s="8"/>
       <c r="W44" s="8"/>
@@ -23421,7 +23427,7 @@
         <v>293</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G45" s="29" t="n">
         <v>1</v>
@@ -23464,7 +23470,7 @@
         <v>46</v>
       </c>
       <c r="U45" s="8" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="V45" s="8"/>
       <c r="W45" s="8"/>
@@ -23526,7 +23532,7 @@
         <v>300</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G46" s="29" t="n">
         <v>1</v>
@@ -23569,7 +23575,7 @@
         <v>46</v>
       </c>
       <c r="U46" s="8" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="V46" s="8"/>
       <c r="W46" s="8"/>
@@ -23631,7 +23637,7 @@
         <v>306</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G47" s="34" t="n">
         <v>1</v>
@@ -23674,7 +23680,7 @@
         <v>150</v>
       </c>
       <c r="U47" s="19" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="V47" s="19"/>
       <c r="W47" s="20"/>
@@ -23736,7 +23742,7 @@
         <v>309</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G48" s="34" t="n">
         <v>1</v>
@@ -23779,7 +23785,7 @@
         <v>150</v>
       </c>
       <c r="U48" s="19" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="V48" s="19"/>
       <c r="W48" s="20"/>
@@ -23841,7 +23847,7 @@
         <v>312</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G49" s="34" t="n">
         <v>1</v>
@@ -23884,7 +23890,7 @@
         <v>150</v>
       </c>
       <c r="U49" s="19" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="V49" s="19"/>
       <c r="W49" s="20"/>
@@ -23946,7 +23952,7 @@
         <v>315</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G50" s="34" t="n">
         <v>1</v>
@@ -23989,7 +23995,7 @@
         <v>150</v>
       </c>
       <c r="U50" s="19" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="V50" s="19"/>
       <c r="W50" s="20"/>
@@ -24051,7 +24057,7 @@
         <v>318</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G51" s="34" t="n">
         <v>1</v>
@@ -24094,7 +24100,7 @@
         <v>150</v>
       </c>
       <c r="U51" s="19" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="V51" s="19"/>
       <c r="W51" s="20"/>
@@ -24156,7 +24162,7 @@
         <v>323</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G52" s="34" t="n">
         <v>1</v>
@@ -24199,7 +24205,7 @@
         <v>150</v>
       </c>
       <c r="U52" s="19" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="V52" s="19"/>
       <c r="W52" s="20"/>
@@ -24261,7 +24267,7 @@
         <v>327</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G53" s="34" t="n">
         <v>1</v>
@@ -24304,7 +24310,7 @@
         <v>150</v>
       </c>
       <c r="U53" s="19" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="V53" s="19"/>
       <c r="W53" s="20"/>
@@ -24366,7 +24372,7 @@
         <v>330</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G54" s="34" t="n">
         <v>1</v>
@@ -24409,7 +24415,7 @@
         <v>150</v>
       </c>
       <c r="U54" s="19" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="V54" s="19"/>
       <c r="W54" s="20"/>
@@ -24471,7 +24477,7 @@
         <v>333</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="G55" s="34" t="n">
         <v>1</v>
@@ -24514,7 +24520,7 @@
         <v>150</v>
       </c>
       <c r="U55" s="19" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="V55" s="19"/>
       <c r="W55" s="20"/>
@@ -24669,7 +24675,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B57" s="76" t="n">
         <v>0</v>
@@ -24710,7 +24716,7 @@
         <v>251</v>
       </c>
       <c r="P57" s="11" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="Q57" s="11" t="s">
         <v>34</v>
@@ -24732,7 +24738,7 @@
         <v>343</v>
       </c>
       <c r="X57" s="11" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="Y57" s="11" t="s">
         <v>345</v>
@@ -24885,7 +24891,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="11" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="B59" s="76" t="n">
         <v>0</v>
@@ -24948,7 +24954,7 @@
         <v>343</v>
       </c>
       <c r="X59" s="11" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="Y59" s="11" t="s">
         <v>345</v>
@@ -25574,7 +25580,7 @@
         <v>221</v>
       </c>
       <c r="P65" s="20" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="Q65" s="34" t="s">
         <v>34</v>
@@ -25596,7 +25602,7 @@
         <v>47</v>
       </c>
       <c r="X65" s="20" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="Y65" s="19" t="s">
         <v>374</v>
@@ -25682,7 +25688,7 @@
         <v>204</v>
       </c>
       <c r="P66" s="20" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="Q66" s="34" t="s">
         <v>34</v>
@@ -25704,7 +25710,7 @@
         <v>47</v>
       </c>
       <c r="X66" s="20" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="Y66" s="19" t="s">
         <v>374</v>
@@ -25790,7 +25796,7 @@
         <v>234</v>
       </c>
       <c r="P67" s="20" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="Q67" s="34" t="s">
         <v>34</v>
@@ -25812,7 +25818,7 @@
         <v>47</v>
       </c>
       <c r="X67" s="20" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="Y67" s="19" t="s">
         <v>374</v>
@@ -25898,7 +25904,7 @@
         <v>221</v>
       </c>
       <c r="P68" s="20" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="Q68" s="34" t="s">
         <v>34</v>
@@ -25920,7 +25926,7 @@
         <v>47</v>
       </c>
       <c r="X68" s="20" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="Y68" s="19" t="s">
         <v>374</v>
@@ -26006,7 +26012,7 @@
         <v>204</v>
       </c>
       <c r="P69" s="20" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="Q69" s="34" t="s">
         <v>34</v>
@@ -26028,7 +26034,7 @@
         <v>47</v>
       </c>
       <c r="X69" s="20" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="Y69" s="19" t="s">
         <v>374</v>
@@ -26114,7 +26120,7 @@
         <v>234</v>
       </c>
       <c r="P70" s="20" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="Q70" s="34" t="s">
         <v>34</v>
@@ -26136,7 +26142,7 @@
         <v>47</v>
       </c>
       <c r="X70" s="20" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="Y70" s="19" t="s">
         <v>374</v>
@@ -26353,7 +26359,7 @@
         <v>59</v>
       </c>
       <c r="U72" s="11" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="V72" s="11"/>
       <c r="W72" s="41"/>
@@ -26397,7 +26403,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="20" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B73" s="22" t="n">
         <v>0</v>
@@ -26442,7 +26448,7 @@
         <v>436</v>
       </c>
       <c r="P73" s="20" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="Q73" s="34" t="s">
         <v>284</v>
@@ -26457,7 +26463,7 @@
         <v>150</v>
       </c>
       <c r="U73" s="19" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="V73" s="19"/>
       <c r="W73" s="44"/>
@@ -26501,7 +26507,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="20" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="B74" s="22" t="n">
         <v>0</v>
@@ -26546,7 +26552,7 @@
         <v>446</v>
       </c>
       <c r="P74" s="20" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="Q74" s="34" t="s">
         <v>284</v>
@@ -26561,7 +26567,7 @@
         <v>150</v>
       </c>
       <c r="U74" s="19" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="V74" s="19"/>
       <c r="W74" s="44"/>
@@ -26605,7 +26611,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="20" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B75" s="22" t="n">
         <v>0</v>
@@ -26650,7 +26656,7 @@
         <v>450</v>
       </c>
       <c r="P75" s="20" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="Q75" s="34" t="s">
         <v>284</v>
@@ -26665,7 +26671,7 @@
         <v>150</v>
       </c>
       <c r="U75" s="19" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="V75" s="19"/>
       <c r="W75" s="44"/>
@@ -27149,7 +27155,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="11" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="B80" s="14" t="n">
         <v>1</v>
@@ -27164,7 +27170,7 @@
         <v>472</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>739</v>
+        <v>855</v>
       </c>
       <c r="G80" s="11" t="s">
         <v>57</v>
@@ -27194,7 +27200,7 @@
         <v>116</v>
       </c>
       <c r="P80" s="11" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="Q80" s="11" t="s">
         <v>476</v>
@@ -27253,7 +27259,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="20" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="B81" s="22" t="n">
         <v>1</v>
@@ -27268,7 +27274,7 @@
         <v>482</v>
       </c>
       <c r="F81" s="20" t="s">
-        <v>739</v>
+        <v>855</v>
       </c>
       <c r="G81" s="20" t="s">
         <v>57</v>
@@ -27298,7 +27304,7 @@
         <v>116</v>
       </c>
       <c r="P81" s="20" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="Q81" s="20" t="s">
         <v>476</v>
@@ -27357,7 +27363,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="11" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="B82" s="14" t="n">
         <v>1</v>
@@ -27372,7 +27378,7 @@
         <v>485</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>739</v>
+        <v>855</v>
       </c>
       <c r="G82" s="11" t="s">
         <v>57</v>
@@ -27402,7 +27408,7 @@
         <v>116</v>
       </c>
       <c r="P82" s="11" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="Q82" s="11" t="s">
         <v>476</v>
@@ -27461,7 +27467,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="20" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="B83" s="22" t="n">
         <v>1</v>
@@ -27476,7 +27482,7 @@
         <v>492</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>739</v>
+        <v>855</v>
       </c>
       <c r="G83" s="20" t="s">
         <v>57</v>
@@ -27506,7 +27512,7 @@
         <v>116</v>
       </c>
       <c r="P83" s="20" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="Q83" s="20" t="s">
         <v>476</v>
@@ -27565,7 +27571,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="11" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="B84" s="14" t="n">
         <v>1</v>
@@ -27580,7 +27586,7 @@
         <v>495</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>739</v>
+        <v>855</v>
       </c>
       <c r="G84" s="11" t="s">
         <v>57</v>
@@ -27625,7 +27631,7 @@
         <v>59</v>
       </c>
       <c r="U84" s="11" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="V84" s="11"/>
       <c r="W84" s="11"/>
@@ -28365,7 +28371,7 @@
         <v>46</v>
       </c>
       <c r="U91" s="8" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="V91" s="15"/>
       <c r="W91" s="15"/>
@@ -28469,7 +28475,7 @@
         <v>46</v>
       </c>
       <c r="U92" s="8" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="V92" s="15"/>
       <c r="W92" s="15"/>
@@ -28513,7 +28519,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="15" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="B93" s="17" t="n">
         <v>1</v>
@@ -28558,7 +28564,7 @@
         <v>522</v>
       </c>
       <c r="P93" s="15" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="Q93" s="29" t="s">
         <v>34</v>
@@ -28573,7 +28579,7 @@
         <v>46</v>
       </c>
       <c r="U93" s="8" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="V93" s="15"/>
       <c r="W93" s="15"/>
@@ -28677,7 +28683,7 @@
         <v>150</v>
       </c>
       <c r="U94" s="19" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="V94" s="20"/>
       <c r="W94" s="20"/>
@@ -28781,7 +28787,7 @@
         <v>46</v>
       </c>
       <c r="U95" s="8" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="V95" s="15"/>
       <c r="W95" s="15"/>
@@ -28885,7 +28891,7 @@
         <v>46</v>
       </c>
       <c r="U96" s="8" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="V96" s="15"/>
       <c r="W96" s="15"/>
@@ -28944,7 +28950,7 @@
         <v>565</v>
       </c>
       <c r="F97" s="15" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="G97" s="15" t="s">
         <v>65</v>
@@ -28977,10 +28983,10 @@
         <v>568</v>
       </c>
       <c r="Q97" s="15" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="R97" s="39" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="S97" s="15" t="s">
         <v>570</v>
@@ -28989,7 +28995,7 @@
         <v>46</v>
       </c>
       <c r="U97" s="8" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="V97" s="15"/>
       <c r="W97" s="15"/>
@@ -29048,7 +29054,7 @@
         <v>575</v>
       </c>
       <c r="F98" s="15" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="G98" s="15" t="s">
         <v>65</v>
@@ -29081,7 +29087,7 @@
         <v>577</v>
       </c>
       <c r="Q98" s="15" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="R98" s="15" t="s">
         <v>525</v>
@@ -29093,7 +29099,7 @@
         <v>46</v>
       </c>
       <c r="U98" s="8" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="V98" s="15"/>
       <c r="W98" s="15"/>
@@ -29357,7 +29363,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="20" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="B101" s="77" t="n">
         <v>0</v>
@@ -29422,7 +29428,7 @@
         <v>585</v>
       </c>
       <c r="X101" s="20" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="Y101" s="20" t="s">
         <v>587</v>
@@ -29687,7 +29693,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="20" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="B104" s="77" t="n">
         <v>0</v>
@@ -29752,7 +29758,7 @@
         <v>585</v>
       </c>
       <c r="X104" s="20" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="Y104" s="20" t="s">
         <v>587</v>
@@ -30017,7 +30023,7 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="11" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="B107" s="14" t="n">
         <v>0</v>
@@ -30060,7 +30066,7 @@
         <v>612</v>
       </c>
       <c r="P107" s="11" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="Q107" s="11" t="s">
         <v>569</v>
@@ -30082,7 +30088,7 @@
         <v>251</v>
       </c>
       <c r="X107" s="11" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="Y107" s="11" t="s">
         <v>51</v>
@@ -30348,7 +30354,7 @@
         <v>635</v>
       </c>
       <c r="F110" s="60" t="s">
-        <v>739</v>
+        <v>855</v>
       </c>
       <c r="G110" s="60" t="n">
         <v>1</v>
@@ -31663,7 +31669,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="20" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="B123" s="22" t="n">
         <v>0</v>
@@ -31765,7 +31771,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="20" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="B124" s="22" t="n">
         <v>0</v>
@@ -32106,7 +32112,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="122.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="81" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="C1" s="81"/>
       <c r="D1" s="81"/>
@@ -32115,200 +32121,200 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="82" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="C2" s="82" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="D2" s="82" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="E2" s="82" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="F2" s="83" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="79" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="B3" s="84" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="84"/>
       <c r="D3" s="84" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="E3" s="84" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="F3" s="85" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="79" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="B4" s="84" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="84"/>
       <c r="D4" s="84" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="E4" s="84"/>
       <c r="F4" s="85" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="79" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="B5" s="84" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="C5" s="84"/>
       <c r="D5" s="86" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="E5" s="84" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="F5" s="87" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="79" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="B6" s="84" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="84"/>
       <c r="D6" s="84" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="E6" s="84"/>
       <c r="F6" s="85" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="79" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="B7" s="84" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="84"/>
       <c r="D7" s="84" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="E7" s="84"/>
       <c r="F7" s="85"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="79" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="B8" s="84" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="C8" s="84"/>
       <c r="D8" s="84" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="E8" s="84"/>
       <c r="F8" s="85"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="79" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="B9" s="84" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="84"/>
       <c r="D9" s="84" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="E9" s="84"/>
       <c r="F9" s="85"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="79" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="B10" s="84" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="C10" s="84"/>
       <c r="D10" s="84" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="E10" s="84"/>
       <c r="F10" s="85" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="79" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="B11" s="84" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="84"/>
       <c r="D11" s="84" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="E11" s="84"/>
       <c r="F11" s="85" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="79" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="B12" s="84" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="C12" s="84"/>
       <c r="D12" s="84" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="E12" s="84"/>
       <c r="F12" s="85"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="79" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="B13" s="84" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="84" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="D13" s="86" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="E13" s="84" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="F13" s="87" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="79" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="B14" s="88" t="s">
         <v>12</v>
@@ -32320,155 +32326,155 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="79" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="B15" s="84" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="84"/>
       <c r="D15" s="84" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="E15" s="84"/>
       <c r="F15" s="87" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="79" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="B16" s="84" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="84"/>
       <c r="D16" s="86" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="E16" s="84"/>
       <c r="F16" s="87" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="79" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="B17" s="84" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="84"/>
       <c r="D17" s="86" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="E17" s="84"/>
       <c r="F17" s="87" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="79" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="B18" s="84" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="84"/>
       <c r="D18" s="84" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="E18" s="84"/>
       <c r="F18" s="85" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="79" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="B19" s="84" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="84"/>
       <c r="D19" s="86" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="E19" s="84"/>
       <c r="F19" s="87" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="79" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="B20" s="84" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="84"/>
       <c r="D20" s="84" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="E20" s="84"/>
       <c r="F20" s="85" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="79" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="B21" s="84" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="84"/>
       <c r="D21" s="86" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="E21" s="84"/>
       <c r="F21" s="85" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="79" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="B22" s="84" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="89" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="D22" s="84"/>
       <c r="E22" s="84" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="F22" s="85" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="79" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="B23" s="84" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="89"/>
       <c r="D23" s="86" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="E23" s="84" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="F23" s="87" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="79" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="B24" s="84" t="s">
         <v>22</v>
@@ -32476,83 +32482,83 @@
       <c r="C24" s="89"/>
       <c r="D24" s="84"/>
       <c r="E24" s="84" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="F24" s="87" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="90" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="B25" s="84" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="89"/>
       <c r="D25" s="86" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="E25" s="84" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="F25" s="87" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="79" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="B26" s="84" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="89"/>
       <c r="D26" s="84" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="E26" s="84"/>
       <c r="F26" s="85"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="79" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="B27" s="84" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="89" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="D27" s="84" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="E27" s="85" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="F27" s="85" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="79" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="B28" s="84" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="C28" s="89"/>
       <c r="D28" s="84" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E28" s="85"/>
       <c r="F28" s="85" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="79" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B29" s="84" t="s">
         <v>27</v>
@@ -32561,12 +32567,12 @@
       <c r="D29" s="84"/>
       <c r="E29" s="85"/>
       <c r="F29" s="85" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="79" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="B30" s="84" t="s">
         <v>28</v>
@@ -32575,30 +32581,30 @@
       <c r="D30" s="84"/>
       <c r="E30" s="85"/>
       <c r="F30" s="85" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="79" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="B31" s="84" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="84"/>
       <c r="D31" s="84" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="E31" s="84" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="F31" s="89" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B32" s="84" t="s">
         <v>30</v>
@@ -32607,12 +32613,12 @@
       <c r="D32" s="84"/>
       <c r="E32" s="84"/>
       <c r="F32" s="89" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="B33" s="84" t="s">
         <v>31</v>
@@ -32621,12 +32627,12 @@
       <c r="D33" s="84"/>
       <c r="E33" s="84"/>
       <c r="F33" s="89" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="B34" s="84" t="s">
         <v>32</v>
@@ -32635,7 +32641,7 @@
       <c r="D34" s="84"/>
       <c r="E34" s="84"/>
       <c r="F34" s="89" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
     </row>
   </sheetData>
@@ -32683,44 +32689,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="91" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="B1" s="91" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="C1" s="91" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="D1" s="91" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="E1" s="91" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="90" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="B2" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="90" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="B3" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>45</v>
@@ -32728,13 +32734,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="90" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="B4" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>45</v>
@@ -32742,13 +32748,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="90" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="B5" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>477</v>
@@ -32756,13 +32762,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="90" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="B6" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>45</v>
@@ -32770,13 +32776,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="90" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="B7" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>45</v>
@@ -32784,13 +32790,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="90" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B8" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>45</v>
@@ -32798,30 +32804,30 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="90" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="B9" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="D9" s="92" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="E9" s="92" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="90" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="B10" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>45</v>
@@ -32829,13 +32835,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="90" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="B11" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>45</v>
@@ -32843,13 +32849,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="90" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="B12" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>45</v>
@@ -32857,58 +32863,58 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="90" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="B13" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="90" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="B14" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="90" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="B15" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>45</v>
       </c>
       <c r="E15" s="93" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="90" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="B16" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>45</v>
@@ -32917,13 +32923,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="90" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="B17" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>45</v>
@@ -32932,13 +32938,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="90" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="B18" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>45</v>
@@ -32947,41 +32953,41 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="90" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="B19" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="90" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="B20" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E20" s="93" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="90" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="B21" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>45</v>
@@ -32990,13 +32996,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="90" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B22" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>45</v>
@@ -33005,13 +33011,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="90" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="B23" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>45</v>
@@ -33019,57 +33025,57 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="90" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="B24" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="90" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="B25" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="90" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="B26" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="90" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="B27" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="90" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="B28" s="90" t="n">
         <v>0</v>
@@ -33078,18 +33084,18 @@
         <v>661</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="90" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="B29" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>45</v>
@@ -33097,13 +33103,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="90" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="B30" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>45</v>
@@ -33111,13 +33117,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="90" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="B31" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>45</v>
@@ -33125,13 +33131,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="90" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="B32" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>45</v>
@@ -33139,13 +33145,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="90" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="B33" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>45</v>
@@ -33153,13 +33159,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="90" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="B34" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>45</v>
@@ -33167,41 +33173,41 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="90" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="B35" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="90" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="B36" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="90" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="B37" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>45</v>
@@ -33209,13 +33215,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="90" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="B38" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>372</v>
@@ -33223,21 +33229,21 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="90" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="B39" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="90" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="B40" s="90" t="n">
         <v>1</v>
@@ -33251,13 +33257,13 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="90" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="B41" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>45</v>
@@ -33265,27 +33271,27 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="90" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="B42" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="90" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="B43" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>45</v>
@@ -33293,13 +33299,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="90" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="B44" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>45</v>
@@ -33307,13 +33313,13 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="90" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="B45" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>45</v>
@@ -33321,13 +33327,13 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="90" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="B46" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>570</v>
@@ -33335,13 +33341,13 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="90" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="B47" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>570</v>
@@ -33349,13 +33355,13 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="90" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="B48" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>45</v>
@@ -33363,13 +33369,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="90" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="B49" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>372</v>
@@ -33377,13 +33383,13 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="90" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
       <c r="B50" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>45</v>
@@ -33391,13 +33397,13 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="90" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
       <c r="B51" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>372</v>
@@ -33405,13 +33411,13 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="90" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
       <c r="B52" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>45</v>
@@ -33419,13 +33425,13 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="90" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
       <c r="B53" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>372</v>
@@ -33433,27 +33439,27 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="90" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="B54" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="90" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="B55" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>45</v>
@@ -33461,13 +33467,13 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="90" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
       <c r="B56" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>45</v>
@@ -33475,13 +33481,13 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="90" t="s">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c r="B57" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>45</v>
@@ -33489,27 +33495,27 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="90" t="s">
-        <v>1094</v>
+        <v>1096</v>
       </c>
       <c r="B58" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="90" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
       <c r="B59" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>372</v>
@@ -33517,111 +33523,111 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="90" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
       <c r="B60" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="90" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="B61" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="90" t="s">
-        <v>1103</v>
+        <v>1105</v>
       </c>
       <c r="B62" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>1104</v>
+        <v>1106</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="90" t="s">
-        <v>1105</v>
+        <v>1107</v>
       </c>
       <c r="B63" s="90" t="n">
         <v>2</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>1106</v>
+        <v>1108</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="90" t="s">
-        <v>1107</v>
+        <v>1109</v>
       </c>
       <c r="B64" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>1108</v>
+        <v>1110</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="90" t="s">
-        <v>1109</v>
+        <v>1111</v>
       </c>
       <c r="B65" s="90" t="n">
         <v>0</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>1110</v>
+        <v>1112</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="90" t="s">
-        <v>1111</v>
+        <v>1113</v>
       </c>
       <c r="B66" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="90" t="s">
-        <v>1114</v>
+        <v>1116</v>
       </c>
       <c r="B67" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>1115</v>
+        <v>1117</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>45</v>
@@ -33629,13 +33635,13 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="90" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="B68" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>45</v>
@@ -33643,27 +33649,27 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="90" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="B69" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="90" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
       <c r="B70" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>1121</v>
+        <v>1123</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>45</v>
@@ -33671,13 +33677,13 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="90" t="s">
-        <v>1122</v>
+        <v>1124</v>
       </c>
       <c r="B71" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>45</v>
@@ -33685,13 +33691,13 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="90" t="s">
-        <v>1124</v>
+        <v>1126</v>
       </c>
       <c r="B72" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>1125</v>
+        <v>1127</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>45</v>
@@ -33699,13 +33705,13 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="90" t="s">
-        <v>1126</v>
+        <v>1128</v>
       </c>
       <c r="B73" s="90" t="n">
         <v>1</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>1127</v>
+        <v>1129</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
fixes #1 and #2
</commit_message>
<xml_diff>
--- a/climate_indices_CV22.xlsx
+++ b/climate_indices_CV22.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7708" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7708" uniqueCount="1132">
   <si>
     <t xml:space="preserve">VarName</t>
   </si>
@@ -2737,10 +2737,10 @@
     <t xml:space="preserve">threshold: (var_name: threshold, standard_name: air_temperature, value: 5, unit: degree_Celsius), condition: &gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">threshold: (var_name: threshold, standard_name:lwe_thickness_of_precipitation_amount, value: 10, unit: mm day-1), condition: &gt;=</t>
-  </si>
-  <si>
-    <t xml:space="preserve">threshold: (var_name: threshold, standard_name:lwe_thickness_of_precipitation_amount, value: 20, unit: mm day-1), condition: &gt;=</t>
+    <t xml:space="preserve">threshold: (var_name: threshold, standard_name: lwe_precipitation_rate, value: 10, unit: mm day-1), condition: &gt;=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">threshold: (var_name: threshold, standard_name: lwe_precipitation_rate, value: 20, unit: mm day-1), condition: &gt;=</t>
   </si>
   <si>
     <t xml:space="preserve">r{RT}mm</t>
@@ -2749,31 +2749,34 @@
     <t xml:space="preserve">Number of days with daily Precip &gt;= {RT}mm)</t>
   </si>
   <si>
-    <t xml:space="preserve">threshold: (var_name: threshold, standard_name:lwe_thickness_of_precipitation_amount, value: {RT}, unit: mm day-1), condition: &gt;=</t>
-  </si>
-  <si>
-    <t xml:space="preserve">threshold: (var_name: threshold, standard_name:lwe_thickness_of_precipitation_amount, value: 1, unit: mm day-1), condition: &gt;=</t>
-  </si>
-  <si>
-    <t xml:space="preserve">threshold: (var_name: threshold, standard_name:lwe_thickness_of_precipitation_amount, value: 1, unit: mm day-1), condition: &lt;, reducer: maximum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">threshold: (var_name: threshold, standard_name:lwe_thickness_of_precipitation_amount, value: 1, unit: mm day-1, condition: &gt;=, reducer: maximum</t>
+    <t xml:space="preserve">threshold: (var_name: threshold, standard_name: lwe_precipitation_rate, value: {RT}, unit: mm day-1), condition: &gt;=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">threshold: (var_name: threshold, standard_name: lwe_precipitation_rate, value: 1, unit: mm day-1), condition: &gt;=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">threshold: (var_name: threshold, standard_name: lwe_precipitation_rate, value: 1, unit: mm day-1), condition: &lt;, reducer: maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">threshold: (var_name: threshold, standard_name: lwe_precipitation_rate, value: 1, unit: mm day-1, condition: &gt;=, reducer: maximum</t>
   </si>
   <si>
     <t xml:space="preserve">thresholded_statistics</t>
   </si>
   <si>
+    <t xml:space="preserve">lwe_precipitation_rate</t>
+  </si>
+  <si>
     <t xml:space="preserve">meter second-1</t>
   </si>
   <si>
     <t xml:space="preserve">mm FREQ-1</t>
   </si>
   <si>
-    <t xml:space="preserve">threshold: (var_name: threshold, standard_name:lwe_thickness_of_precipitation_amount, value: 1, unit: mm day-1), condition: &gt;=, reducer: sum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">threshold: (var_name: threshold, standard_name:lwe_thickness_of_precipitation_amount, value: 1, unit: mm day-1), condition: &gt;=, reducer: mean</t>
+    <t xml:space="preserve">threshold: (var_name: threshold, standard_name: lwe_precipitation_rate, value: 1, unit: mm day-1), condition: &gt;=, reducer: sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">threshold: (var_name: threshold, standard_name: lwe_precipitation_rate, value: 1, unit: mm day-1), condition: &gt;=, reducer: mean</t>
   </si>
   <si>
     <t xml:space="preserve">r{PRC}ptot</t>
@@ -18767,7 +18770,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A67" activeCellId="0" sqref="A67"/>
-      <selection pane="bottomRight" activeCell="R97" activeCellId="0" sqref="R97"/>
+      <selection pane="bottomRight" activeCell="A97" activeCellId="0" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -28983,7 +28986,7 @@
         <v>39</v>
       </c>
       <c r="L97" s="15" t="s">
-        <v>524</v>
+        <v>875</v>
       </c>
       <c r="M97" s="8" t="s">
         <v>41</v>
@@ -28998,10 +29001,10 @@
         <v>568</v>
       </c>
       <c r="Q97" s="15" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="R97" s="80" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="S97" s="15" t="s">
         <v>570</v>
@@ -29010,7 +29013,7 @@
         <v>46</v>
       </c>
       <c r="U97" s="8" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="V97" s="15"/>
       <c r="W97" s="15"/>
@@ -29087,7 +29090,7 @@
         <v>39</v>
       </c>
       <c r="L98" s="15" t="s">
-        <v>524</v>
+        <v>875</v>
       </c>
       <c r="M98" s="8" t="s">
         <v>41</v>
@@ -29102,7 +29105,7 @@
         <v>577</v>
       </c>
       <c r="Q98" s="15" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="R98" s="15" t="s">
         <v>525</v>
@@ -29114,7 +29117,7 @@
         <v>46</v>
       </c>
       <c r="U98" s="8" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="V98" s="15"/>
       <c r="W98" s="15"/>
@@ -29378,7 +29381,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="20" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B101" s="78" t="n">
         <v>0</v>
@@ -29443,7 +29446,7 @@
         <v>585</v>
       </c>
       <c r="X101" s="20" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="Y101" s="20" t="s">
         <v>587</v>
@@ -29708,7 +29711,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="20" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B104" s="78" t="n">
         <v>0</v>
@@ -29773,7 +29776,7 @@
         <v>585</v>
       </c>
       <c r="X104" s="20" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="Y104" s="20" t="s">
         <v>587</v>
@@ -30038,7 +30041,7 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="11" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B107" s="14" t="n">
         <v>0</v>
@@ -30081,7 +30084,7 @@
         <v>612</v>
       </c>
       <c r="P107" s="11" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="Q107" s="11" t="s">
         <v>569</v>
@@ -30103,7 +30106,7 @@
         <v>251</v>
       </c>
       <c r="X107" s="11" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="Y107" s="11" t="s">
         <v>51</v>
@@ -31684,7 +31687,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="20" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="B123" s="22" t="n">
         <v>0</v>
@@ -31786,7 +31789,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="20" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B124" s="22" t="n">
         <v>0</v>
@@ -32127,7 +32130,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="122.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="84" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="C1" s="84"/>
       <c r="D1" s="84"/>
@@ -32136,200 +32139,200 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="85" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C2" s="85" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="D2" s="85" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="E2" s="85" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="F2" s="86" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="82" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B3" s="87" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="87"/>
       <c r="D3" s="87" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="E3" s="87" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="F3" s="88" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="82" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B4" s="87" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="87"/>
       <c r="D4" s="87" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="E4" s="87"/>
       <c r="F4" s="88" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="82" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B5" s="87" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C5" s="87"/>
       <c r="D5" s="89" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="E5" s="87" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="F5" s="90" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="82" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="B6" s="87" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="87"/>
       <c r="D6" s="87" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="E6" s="87"/>
       <c r="F6" s="88" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="82" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B7" s="87" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="87"/>
       <c r="D7" s="87" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="E7" s="87"/>
       <c r="F7" s="88"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="82" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="B8" s="87" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="C8" s="87"/>
       <c r="D8" s="87" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="E8" s="87"/>
       <c r="F8" s="88"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="82" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B9" s="87" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="87"/>
       <c r="D9" s="87" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="E9" s="87"/>
       <c r="F9" s="88"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="82" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="B10" s="87" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="C10" s="87"/>
       <c r="D10" s="87" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="E10" s="87"/>
       <c r="F10" s="88" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="82" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="B11" s="87" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="87"/>
       <c r="D11" s="87" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="E11" s="87"/>
       <c r="F11" s="88" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="82" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="B12" s="87" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="C12" s="87"/>
       <c r="D12" s="87" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="E12" s="87"/>
       <c r="F12" s="88"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="82" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="B13" s="87" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="87" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="D13" s="89" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="E13" s="87" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="F13" s="90" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="82" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="B14" s="91" t="s">
         <v>12</v>
@@ -32341,155 +32344,155 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="82" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B15" s="87" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="87"/>
       <c r="D15" s="87" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="E15" s="87"/>
       <c r="F15" s="90" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="82" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B16" s="87" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="87"/>
       <c r="D16" s="89" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="E16" s="87"/>
       <c r="F16" s="90" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="82" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="B17" s="87" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="87"/>
       <c r="D17" s="89" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="E17" s="87"/>
       <c r="F17" s="90" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="82" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B18" s="87" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="87"/>
       <c r="D18" s="87" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="E18" s="87"/>
       <c r="F18" s="88" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="82" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B19" s="87" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="87"/>
       <c r="D19" s="89" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="E19" s="87"/>
       <c r="F19" s="90" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="82" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="B20" s="87" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="87"/>
       <c r="D20" s="87" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="E20" s="87"/>
       <c r="F20" s="88" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="82" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="B21" s="87" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="87"/>
       <c r="D21" s="89" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="E21" s="87"/>
       <c r="F21" s="88" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="82" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B22" s="87" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="92" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="D22" s="87"/>
       <c r="E22" s="87" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="F22" s="88" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="82" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B23" s="87" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="92"/>
       <c r="D23" s="89" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="E23" s="87" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="F23" s="90" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="82" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B24" s="87" t="s">
         <v>22</v>
@@ -32497,83 +32500,83 @@
       <c r="C24" s="92"/>
       <c r="D24" s="87"/>
       <c r="E24" s="87" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="F24" s="90" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="93" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="B25" s="87" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="92"/>
       <c r="D25" s="89" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="E25" s="87" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="F25" s="90" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="82" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="B26" s="87" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="92"/>
       <c r="D26" s="87" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="E26" s="87"/>
       <c r="F26" s="88"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="82" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B27" s="87" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="92" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="D27" s="87" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="E27" s="88" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="F27" s="88" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="82" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B28" s="87" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C28" s="92"/>
       <c r="D28" s="87" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="E28" s="88"/>
       <c r="F28" s="88" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="82" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B29" s="87" t="s">
         <v>27</v>
@@ -32582,12 +32585,12 @@
       <c r="D29" s="87"/>
       <c r="E29" s="88"/>
       <c r="F29" s="88" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="82" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B30" s="87" t="s">
         <v>28</v>
@@ -32596,30 +32599,30 @@
       <c r="D30" s="87"/>
       <c r="E30" s="88"/>
       <c r="F30" s="88" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="82" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="B31" s="87" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="87"/>
       <c r="D31" s="87" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="E31" s="87" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="F31" s="92" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B32" s="87" t="s">
         <v>30</v>
@@ -32628,12 +32631,12 @@
       <c r="D32" s="87"/>
       <c r="E32" s="87"/>
       <c r="F32" s="92" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B33" s="87" t="s">
         <v>31</v>
@@ -32642,12 +32645,12 @@
       <c r="D33" s="87"/>
       <c r="E33" s="87"/>
       <c r="F33" s="92" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="B34" s="87" t="s">
         <v>32</v>
@@ -32656,7 +32659,7 @@
       <c r="D34" s="87"/>
       <c r="E34" s="87"/>
       <c r="F34" s="92" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
   </sheetData>
@@ -32704,44 +32707,44 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="94" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="B1" s="94" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="C1" s="94" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="D1" s="94" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="E1" s="94" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="93" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="B2" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="93" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B3" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>45</v>
@@ -32749,13 +32752,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="93" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="B4" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>45</v>
@@ -32763,13 +32766,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="93" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="B5" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>477</v>
@@ -32777,13 +32780,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="93" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B6" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>45</v>
@@ -32791,13 +32794,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="93" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="B7" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>45</v>
@@ -32805,13 +32808,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="93" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B8" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>45</v>
@@ -32819,30 +32822,30 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="93" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B9" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="D9" s="95" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="E9" s="95" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="93" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="B10" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>45</v>
@@ -32850,13 +32853,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="93" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B11" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>45</v>
@@ -32864,13 +32867,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="93" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B12" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>45</v>
@@ -32878,58 +32881,58 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="93" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="B13" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="93" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B14" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="93" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B15" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>45</v>
       </c>
       <c r="E15" s="96" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="93" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B16" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>45</v>
@@ -32938,13 +32941,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="93" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B17" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>45</v>
@@ -32953,13 +32956,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="93" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B18" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>45</v>
@@ -32968,41 +32971,41 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="93" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B19" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="93" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B20" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="E20" s="96" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="93" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="B21" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>45</v>
@@ -33011,13 +33014,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="93" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B22" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>45</v>
@@ -33026,13 +33029,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="93" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B23" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>45</v>
@@ -33040,57 +33043,57 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="93" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B24" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="93" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B25" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="93" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B26" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="93" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B27" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="93" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B28" s="93" t="n">
         <v>0</v>
@@ -33099,18 +33102,18 @@
         <v>661</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="93" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="B29" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>45</v>
@@ -33118,13 +33121,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="93" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="B30" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>45</v>
@@ -33132,13 +33135,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="93" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B31" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>45</v>
@@ -33146,13 +33149,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="93" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="B32" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>45</v>
@@ -33160,13 +33163,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="93" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="B33" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>45</v>
@@ -33174,13 +33177,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="93" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="B34" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>45</v>
@@ -33188,41 +33191,41 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="93" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="B35" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="93" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="B36" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="93" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="B37" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>45</v>
@@ -33230,13 +33233,13 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="93" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="B38" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>372</v>
@@ -33244,21 +33247,21 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="93" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B39" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="93" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="B40" s="93" t="n">
         <v>1</v>
@@ -33272,13 +33275,13 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="93" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="B41" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>45</v>
@@ -33286,27 +33289,27 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="93" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="B42" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="93" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="B43" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>45</v>
@@ -33314,13 +33317,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="93" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="B44" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>45</v>
@@ -33328,13 +33331,13 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="93" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="B45" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>45</v>
@@ -33342,13 +33345,13 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="93" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="B46" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>570</v>
@@ -33356,13 +33359,13 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="93" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="B47" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>570</v>
@@ -33370,13 +33373,13 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="93" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B48" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>45</v>
@@ -33384,13 +33387,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="93" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="B49" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>372</v>
@@ -33398,13 +33401,13 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="93" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="B50" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>45</v>
@@ -33412,13 +33415,13 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="93" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="B51" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>372</v>
@@ -33426,13 +33429,13 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="93" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="B52" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>45</v>
@@ -33440,13 +33443,13 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="93" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="B53" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>372</v>
@@ -33454,27 +33457,27 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="93" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="B54" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="93" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B55" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>45</v>
@@ -33482,13 +33485,13 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="93" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="B56" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>45</v>
@@ -33496,13 +33499,13 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="93" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B57" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>45</v>
@@ -33510,27 +33513,27 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="93" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="B58" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="93" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B59" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>372</v>
@@ -33538,111 +33541,111 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="93" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B60" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="93" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="B61" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="93" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="B62" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="93" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="B63" s="93" t="n">
         <v>2</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="93" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="B64" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="93" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="B65" s="93" t="n">
         <v>0</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="93" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="B66" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="93" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="B67" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>45</v>
@@ -33650,13 +33653,13 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="93" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="B68" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>45</v>
@@ -33664,27 +33667,27 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="93" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="B69" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="93" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="B70" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>45</v>
@@ -33692,13 +33695,13 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="93" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="B71" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>45</v>
@@ -33706,13 +33709,13 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="93" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="B72" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>45</v>
@@ -33720,13 +33723,13 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="93" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="B73" s="93" t="n">
         <v>1</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
fixed errors in N_inputs for txm, tnm, tmx, tmx, and tmm
</commit_message>
<xml_diff>
--- a/climate_indices_CV22.xlsx
+++ b/climate_indices_CV22.xlsx
@@ -18859,11 +18859,11 @@
   <dimension ref="A1:AS131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="R1" activeCellId="0" sqref="R1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
-      <selection pane="bottomRight" activeCell="U48" activeCellId="0" sqref="U48"/>
+      <selection pane="bottomRight" activeCell="I52" activeCellId="0" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23856,7 +23856,7 @@
         <v>765</v>
       </c>
       <c r="I48" s="76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J48" s="79" t="s">
         <v>38</v>
@@ -23955,7 +23955,7 @@
         <v>765</v>
       </c>
       <c r="I49" s="76" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J49" s="79" t="s">
         <v>38</v>
@@ -24054,7 +24054,7 @@
         <v>765</v>
       </c>
       <c r="I50" s="76" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J50" s="79" t="s">
         <v>38</v>
@@ -24153,7 +24153,7 @@
         <v>765</v>
       </c>
       <c r="I51" s="76" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J51" s="79" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
fixed prcptot standardname and output units
</commit_message>
<xml_diff>
--- a/climate_indices_CV22.xlsx
+++ b/climate_indices_CV22.xlsx
@@ -2833,16 +2833,16 @@
     <t xml:space="preserve">thresholded_statistics</t>
   </si>
   <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">threshold: (var_name: threshold, standard_name: lwe_precipitation_rate, value: 1, unit: mm day-1), condition: &gt;=, reducer: sum</t>
+  </si>
+  <si>
     <t xml:space="preserve">lwe_precipitation_rate</t>
   </si>
   <si>
     <t xml:space="preserve">meter second-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mm FREQ-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">threshold: (var_name: threshold, standard_name: lwe_precipitation_rate, value: 1, unit: mm day-1), condition: &gt;=, reducer: sum</t>
   </si>
   <si>
     <t xml:space="preserve">threshold: (var_name: threshold, standard_name: lwe_precipitation_rate, value: 1, unit: mm day-1), condition: &gt;=, reducer: mean</t>
@@ -4267,7 +4267,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -18859,11 +18859,11 @@
   <dimension ref="A1:AS131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M67" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
-      <selection pane="bottomRight" activeCell="I52" activeCellId="0" sqref="I52"/>
+      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="A67" activeCellId="0" sqref="A67"/>
+      <selection pane="bottomRight" activeCell="P102" activeCellId="0" sqref="P102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29574,7 +29574,7 @@
         <v>39</v>
       </c>
       <c r="L102" s="15" t="s">
-        <v>898</v>
+        <v>524</v>
       </c>
       <c r="M102" s="8" t="s">
         <v>41</v>
@@ -29589,10 +29589,10 @@
         <v>568</v>
       </c>
       <c r="Q102" s="15" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="R102" s="86" t="s">
-        <v>900</v>
+        <v>570</v>
       </c>
       <c r="S102" s="15" t="s">
         <v>570</v>
@@ -29601,7 +29601,7 @@
         <v>46</v>
       </c>
       <c r="U102" s="8" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="V102" s="15"/>
       <c r="W102" s="15"/>
@@ -29678,7 +29678,7 @@
         <v>39</v>
       </c>
       <c r="L103" s="15" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="M103" s="8" t="s">
         <v>41</v>
@@ -29693,7 +29693,7 @@
         <v>577</v>
       </c>
       <c r="Q103" s="15" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="R103" s="15" t="s">
         <v>525</v>

</xml_diff>